<commit_message>
algumas alteracoes de textos minimas
</commit_message>
<xml_diff>
--- a/Traduzido/PTBR/Lang/PTBR/Game/General.xlsx
+++ b/Traduzido/PTBR/Lang/PTBR/Game/General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9409C-EDDA-47C6-A665-E91DA018E716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103DA889-BCCA-413B-9788-9C15C2A849D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7875" yWindow="3060" windowWidth="17790" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4485" yWindow="6420" windowWidth="17790" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -43470,9 +43470,6 @@
     <t>Sem Telhado</t>
   </si>
   <si>
-    <t>(+#1 outro(s) item(ns))</t>
-  </si>
-  <si>
     <t>Quarto de #1</t>
   </si>
   <si>
@@ -44979,6 +44976,9 @@
   </si>
   <si>
     <t>&lt;color=#FFFF88&gt;Onda de Inimigos #1 - Nv.#3&lt;/color&gt; (#2 abate#(s))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (+#1 outro(s) item(ns))</t>
   </si>
 </sst>
 </file>
@@ -45171,8 +45171,8 @@
   <dimension ref="A1:F2561"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
+      <pane ySplit="2" topLeftCell="A1680" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1692" sqref="D1692"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5"/>
@@ -45214,7 +45214,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9536</v>
+        <v>9535</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
@@ -45234,7 +45234,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9523</v>
+        <v>9522</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -45254,7 +45254,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9523</v>
+        <v>9522</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>22</v>
@@ -45274,7 +45274,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9526</v>
+        <v>9525</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>29</v>
@@ -45625,7 +45625,7 @@
         <v>1335</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>9471</v>
+        <v>9470</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>8848</v>
@@ -45779,7 +45779,7 @@
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>9468</v>
+        <v>9467</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>54</v>
@@ -46013,7 +46013,7 @@
         <v>8</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>9527</v>
+        <v>9526</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>138</v>
@@ -46124,7 +46124,7 @@
         <v>8</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>9539</v>
+        <v>9538</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>69</v>
@@ -46144,7 +46144,7 @@
         <v>8</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>9469</v>
+        <v>9468</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>22</v>
@@ -46244,7 +46244,7 @@
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9525</v>
+        <v>9524</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>78</v>
@@ -46318,7 +46318,7 @@
         <v>981</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>9528</v>
+        <v>9527</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>982</v>
@@ -46355,7 +46355,7 @@
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>9472</v>
+        <v>9471</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>8854</v>
@@ -46375,7 +46375,7 @@
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>9538</v>
+        <v>9537</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>88</v>
@@ -46503,7 +46503,7 @@
         <v>4753</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>9473</v>
+        <v>9472</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>4754</v>
@@ -46566,7 +46566,7 @@
         <v>106</v>
       </c>
       <c r="F73" t="s">
-        <v>9531</v>
+        <v>9530</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -46605,7 +46605,7 @@
         <v>7</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>9524</v>
+        <v>9523</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>4776</v>
@@ -46625,7 +46625,7 @@
         <v>8</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>9537</v>
+        <v>9536</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>90</v>
@@ -46671,7 +46671,7 @@
         <v>112</v>
       </c>
       <c r="F79" t="s">
-        <v>9530</v>
+        <v>9529</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -46702,7 +46702,7 @@
         <v>108</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>9103</v>
+        <v>9102</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>5585</v>
@@ -46776,7 +46776,7 @@
         <v>2973</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>9394</v>
+        <v>9393</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>7041</v>
@@ -47878,7 +47878,7 @@
         <v>6800</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>9318</v>
+        <v>9317</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>6801</v>
@@ -49129,7 +49129,7 @@
         <v>2626</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>9097</v>
+        <v>9096</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>5564</v>
@@ -49186,7 +49186,7 @@
         <v>2626</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>9412</v>
+        <v>9411</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>7101</v>
@@ -49334,7 +49334,7 @@
         <v>15</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>9435</v>
+        <v>9434</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>7173</v>
@@ -49351,7 +49351,7 @@
         <v>6875</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>9341</v>
+        <v>9340</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>6876</v>
@@ -49442,7 +49442,7 @@
         <v>7</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>9540</v>
+        <v>9539</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>4808</v>
@@ -49610,7 +49610,7 @@
         <v>3085</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>9122</v>
+        <v>9121</v>
       </c>
       <c r="E230" s="1" t="s">
         <v>5650</v>
@@ -50560,7 +50560,7 @@
         <v>6062</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>9477</v>
+        <v>9476</v>
       </c>
       <c r="E279" s="1" t="s">
         <v>6072</v>
@@ -50577,7 +50577,7 @@
         <v>2626</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>9413</v>
+        <v>9412</v>
       </c>
       <c r="E280" s="1" t="s">
         <v>7104</v>
@@ -50977,7 +50977,7 @@
         <v>281</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>9470</v>
+        <v>9469</v>
       </c>
       <c r="E303" s="1" t="s">
         <v>8878</v>
@@ -51171,7 +51171,7 @@
         <v>6038</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>9247</v>
+        <v>9246</v>
       </c>
       <c r="E313" s="1" t="s">
         <v>3595</v>
@@ -51709,7 +51709,7 @@
         <v>6310</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>9469</v>
+        <v>9468</v>
       </c>
       <c r="E342" s="1" t="s">
         <v>6314</v>
@@ -51823,7 +51823,7 @@
         <v>6062</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>9257</v>
+        <v>9256</v>
       </c>
       <c r="E348" s="1" t="s">
         <v>6069</v>
@@ -52173,7 +52173,7 @@
         <v>871</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>9535</v>
+        <v>9534</v>
       </c>
       <c r="E367" s="1" t="s">
         <v>914</v>
@@ -52193,7 +52193,7 @@
         <v>8</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>9529</v>
+        <v>9528</v>
       </c>
       <c r="E368" s="1" t="s">
         <v>155</v>
@@ -52273,7 +52273,7 @@
         <v>6062</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>9256</v>
+        <v>9255</v>
       </c>
       <c r="E372" s="1" t="s">
         <v>6066</v>
@@ -52393,13 +52393,13 @@
         <v>6641</v>
       </c>
       <c r="D378" s="1" t="s">
+        <v>9263</v>
+      </c>
+      <c r="E378" s="1" t="s">
         <v>9264</v>
       </c>
-      <c r="E378" s="1" t="s">
+      <c r="F378" s="1" t="s">
         <v>9265</v>
-      </c>
-      <c r="F378" s="1" t="s">
-        <v>9266</v>
       </c>
     </row>
     <row r="379" spans="1:6">
@@ -52481,7 +52481,7 @@
         <v>6062</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>9255</v>
+        <v>9254</v>
       </c>
       <c r="E383" s="1" t="s">
         <v>6063</v>
@@ -53492,7 +53492,7 @@
         <v>2361</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>9474</v>
+        <v>9473</v>
       </c>
       <c r="E434" s="1" t="s">
         <v>2362</v>
@@ -54296,7 +54296,7 @@
         <v>267</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>9370</v>
+        <v>9369</v>
       </c>
       <c r="E476" s="1" t="s">
         <v>6951</v>
@@ -54313,7 +54313,7 @@
         <v>267</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>9373</v>
+        <v>9372</v>
       </c>
       <c r="E477" s="1" t="s">
         <v>6960</v>
@@ -54330,7 +54330,7 @@
         <v>267</v>
       </c>
       <c r="D478" s="1" t="s">
-        <v>9371</v>
+        <v>9370</v>
       </c>
       <c r="E478" s="1" t="s">
         <v>6954</v>
@@ -54364,7 +54364,7 @@
         <v>267</v>
       </c>
       <c r="D480" s="1" t="s">
-        <v>9372</v>
+        <v>9371</v>
       </c>
       <c r="E480" s="1" t="s">
         <v>6957</v>
@@ -54398,7 +54398,7 @@
         <v>1069</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>9424</v>
+        <v>9423</v>
       </c>
       <c r="E482" s="1" t="s">
         <v>7139</v>
@@ -54623,7 +54623,7 @@
         <v>1035</v>
       </c>
       <c r="D494" s="1" t="s">
-        <v>9374</v>
+        <v>9373</v>
       </c>
       <c r="E494" s="1" t="s">
         <v>6965</v>
@@ -55024,7 +55024,7 @@
         <v>1950</v>
       </c>
       <c r="D516" s="4" t="s">
-        <v>9421</v>
+        <v>9420</v>
       </c>
       <c r="E516" s="4" t="s">
         <v>7130</v>
@@ -55141,7 +55141,7 @@
         <v>2761</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>9478</v>
+        <v>9477</v>
       </c>
       <c r="E522" s="1" t="s">
         <v>8627</v>
@@ -55355,7 +55355,7 @@
         <v>6991</v>
       </c>
       <c r="D533" s="1" t="s">
-        <v>9383</v>
+        <v>9382</v>
       </c>
       <c r="E533" s="1" t="s">
         <v>6992</v>
@@ -55372,7 +55372,7 @@
         <v>7</v>
       </c>
       <c r="D534" s="1" t="s">
-        <v>9479</v>
+        <v>9478</v>
       </c>
       <c r="E534" s="1" t="s">
         <v>4981</v>
@@ -55409,7 +55409,7 @@
         <v>217</v>
       </c>
       <c r="D536" s="1" t="s">
-        <v>9311</v>
+        <v>9310</v>
       </c>
       <c r="E536" s="1" t="s">
         <v>6779</v>
@@ -55446,7 +55446,7 @@
         <v>42</v>
       </c>
       <c r="D538" s="1" t="s">
-        <v>9480</v>
+        <v>9479</v>
       </c>
       <c r="E538" s="1" t="s">
         <v>6131</v>
@@ -55540,7 +55540,7 @@
         <v>710</v>
       </c>
       <c r="D543" s="1" t="s">
-        <v>9346</v>
+        <v>9345</v>
       </c>
       <c r="E543" s="1" t="s">
         <v>6891</v>
@@ -55577,7 +55577,7 @@
         <v>3009</v>
       </c>
       <c r="D545" s="1" t="s">
-        <v>9404</v>
+        <v>9403</v>
       </c>
       <c r="E545" s="1" t="s">
         <v>7073</v>
@@ -55785,7 +55785,7 @@
         <v>1892</v>
       </c>
       <c r="D556" s="1" t="s">
-        <v>9544</v>
+        <v>9543</v>
       </c>
       <c r="E556" s="1" t="s">
         <v>8618</v>
@@ -57481,7 +57481,7 @@
         <v>2197</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>9387</v>
+        <v>9386</v>
       </c>
       <c r="E642" s="1" t="s">
         <v>7005</v>
@@ -57498,7 +57498,7 @@
         <v>2197</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>9388</v>
+        <v>9387</v>
       </c>
       <c r="E643" s="1" t="s">
         <v>7008</v>
@@ -57615,7 +57615,7 @@
         <v>1933</v>
       </c>
       <c r="D649" s="1" t="s">
-        <v>9543</v>
+        <v>9542</v>
       </c>
       <c r="E649" s="1" t="s">
         <v>914</v>
@@ -58082,13 +58082,13 @@
         <v>6641</v>
       </c>
       <c r="D674" s="1" t="s">
-        <v>9545</v>
+        <v>9544</v>
       </c>
       <c r="E674" s="1" t="s">
+        <v>9266</v>
+      </c>
+      <c r="F674" s="1" t="s">
         <v>9267</v>
-      </c>
-      <c r="F674" s="1" t="s">
-        <v>9268</v>
       </c>
     </row>
     <row r="675" spans="1:6">
@@ -58190,7 +58190,7 @@
         <v>462</v>
       </c>
       <c r="D680" s="1" t="s">
-        <v>9407</v>
+        <v>9406</v>
       </c>
       <c r="E680" s="1" t="s">
         <v>7082</v>
@@ -59652,7 +59652,7 @@
         <v>5018</v>
       </c>
       <c r="D754" s="1" t="s">
-        <v>9400</v>
+        <v>9399</v>
       </c>
       <c r="E754" s="1" t="s">
         <v>7061</v>
@@ -59669,7 +59669,7 @@
         <v>5018</v>
       </c>
       <c r="D755" s="1" t="s">
-        <v>9401</v>
+        <v>9400</v>
       </c>
       <c r="E755" s="1" t="s">
         <v>7064</v>
@@ -59686,7 +59686,7 @@
         <v>445</v>
       </c>
       <c r="D756" s="4" t="s">
-        <v>9402</v>
+        <v>9401</v>
       </c>
       <c r="E756" s="4" t="s">
         <v>7067</v>
@@ -59851,7 +59851,7 @@
         <v>7150</v>
       </c>
       <c r="D765" s="1" t="s">
-        <v>9429</v>
+        <v>9428</v>
       </c>
       <c r="E765" s="1" t="s">
         <v>7154</v>
@@ -60010,7 +60010,7 @@
         <v>6038</v>
       </c>
       <c r="D774" s="1" t="s">
-        <v>9252</v>
+        <v>9251</v>
       </c>
       <c r="E774" s="1" t="s">
         <v>6053</v>
@@ -60030,7 +60030,7 @@
         <v>6038</v>
       </c>
       <c r="D775" s="4" t="s">
-        <v>9253</v>
+        <v>9252</v>
       </c>
       <c r="E775" s="4" t="s">
         <v>6056</v>
@@ -60050,7 +60050,7 @@
         <v>6038</v>
       </c>
       <c r="D776" s="1" t="s">
-        <v>9248</v>
+        <v>9247</v>
       </c>
       <c r="E776" s="1" t="s">
         <v>6041</v>
@@ -60070,7 +60070,7 @@
         <v>6038</v>
       </c>
       <c r="D777" s="4" t="s">
-        <v>9249</v>
+        <v>9248</v>
       </c>
       <c r="E777" s="4" t="s">
         <v>6044</v>
@@ -60090,7 +60090,7 @@
         <v>6038</v>
       </c>
       <c r="D778" s="1" t="s">
-        <v>9254</v>
+        <v>9253</v>
       </c>
       <c r="E778" s="1" t="s">
         <v>6059</v>
@@ -60110,7 +60110,7 @@
         <v>6038</v>
       </c>
       <c r="D779" s="1" t="s">
-        <v>9250</v>
+        <v>9249</v>
       </c>
       <c r="E779" s="1" t="s">
         <v>6047</v>
@@ -60130,7 +60130,7 @@
         <v>6038</v>
       </c>
       <c r="D780" s="4" t="s">
-        <v>9251</v>
+        <v>9250</v>
       </c>
       <c r="E780" s="4" t="s">
         <v>6050</v>
@@ -60241,7 +60241,7 @@
         <v>1340</v>
       </c>
       <c r="D786" s="1" t="s">
-        <v>9448</v>
+        <v>9447</v>
       </c>
       <c r="E786" s="1" t="s">
         <v>7216</v>
@@ -61016,7 +61016,7 @@
         <v>256</v>
       </c>
       <c r="D827" s="1" t="s">
-        <v>9426</v>
+        <v>9425</v>
       </c>
       <c r="E827" s="1" t="s">
         <v>7144</v>
@@ -61247,7 +61247,7 @@
         <v>7</v>
       </c>
       <c r="D839" s="1" t="s">
-        <v>9481</v>
+        <v>9480</v>
       </c>
       <c r="E839" s="1" t="s">
         <v>5154</v>
@@ -61267,13 +61267,13 @@
         <v>6641</v>
       </c>
       <c r="D840" s="1" t="s">
+        <v>9271</v>
+      </c>
+      <c r="E840" s="1" t="s">
         <v>9272</v>
       </c>
-      <c r="E840" s="1" t="s">
+      <c r="F840" s="1" t="s">
         <v>9273</v>
-      </c>
-      <c r="F840" s="1" t="s">
-        <v>9274</v>
       </c>
     </row>
     <row r="841" spans="1:6">
@@ -61287,13 +61287,13 @@
         <v>6641</v>
       </c>
       <c r="D841" s="1" t="s">
+        <v>9268</v>
+      </c>
+      <c r="E841" s="1" t="s">
         <v>9269</v>
       </c>
-      <c r="E841" s="1" t="s">
+      <c r="F841" s="1" t="s">
         <v>9270</v>
-      </c>
-      <c r="F841" s="1" t="s">
-        <v>9271</v>
       </c>
     </row>
     <row r="842" spans="1:6">
@@ -61304,7 +61304,7 @@
         <v>5204</v>
       </c>
       <c r="D842" s="1" t="s">
-        <v>9342</v>
+        <v>9341</v>
       </c>
       <c r="E842" s="1" t="s">
         <v>6879</v>
@@ -61321,7 +61321,7 @@
         <v>5204</v>
       </c>
       <c r="D843" s="4" t="s">
-        <v>9343</v>
+        <v>9342</v>
       </c>
       <c r="E843" s="4" t="s">
         <v>6882</v>
@@ -61494,7 +61494,7 @@
         <v>978</v>
       </c>
       <c r="D853" s="1" t="s">
-        <v>9367</v>
+        <v>9366</v>
       </c>
       <c r="E853" s="1" t="s">
         <v>6942</v>
@@ -61970,7 +61970,7 @@
         <v>93</v>
       </c>
       <c r="D878" s="1" t="s">
-        <v>9283</v>
+        <v>9282</v>
       </c>
       <c r="E878" s="1" t="s">
         <v>6688</v>
@@ -61987,7 +61987,7 @@
         <v>93</v>
       </c>
       <c r="D879" s="1" t="s">
-        <v>9282</v>
+        <v>9281</v>
       </c>
       <c r="E879" s="1" t="s">
         <v>6685</v>
@@ -62081,7 +62081,7 @@
         <v>93</v>
       </c>
       <c r="D884" s="1" t="s">
-        <v>9281</v>
+        <v>9280</v>
       </c>
       <c r="E884" s="1" t="s">
         <v>6679</v>
@@ -62098,7 +62098,7 @@
         <v>93</v>
       </c>
       <c r="D885" s="1" t="s">
-        <v>9284</v>
+        <v>9283</v>
       </c>
       <c r="E885" s="1" t="s">
         <v>6691</v>
@@ -62380,13 +62380,13 @@
         <v>6924</v>
       </c>
       <c r="D900" s="1" t="s">
-        <v>9482</v>
+        <v>9481</v>
       </c>
       <c r="E900" s="1" t="s">
+        <v>9357</v>
+      </c>
+      <c r="F900" t="s">
         <v>9358</v>
-      </c>
-      <c r="F900" t="s">
-        <v>9359</v>
       </c>
     </row>
     <row r="901" spans="1:6">
@@ -62397,7 +62397,7 @@
         <v>217</v>
       </c>
       <c r="D901" s="1" t="s">
-        <v>9310</v>
+        <v>9309</v>
       </c>
       <c r="E901" s="1" t="s">
         <v>6776</v>
@@ -62414,13 +62414,13 @@
         <v>3380</v>
       </c>
       <c r="D902" s="1" t="s">
-        <v>9483</v>
+        <v>9482</v>
       </c>
       <c r="E902" s="1" t="s">
+        <v>9359</v>
+      </c>
+      <c r="F902" t="s">
         <v>9360</v>
-      </c>
-      <c r="F902" t="s">
-        <v>9361</v>
       </c>
     </row>
     <row r="903" spans="1:6">
@@ -62431,7 +62431,7 @@
         <v>3380</v>
       </c>
       <c r="D903" s="1" t="s">
-        <v>9362</v>
+        <v>9361</v>
       </c>
       <c r="E903" s="1" t="s">
         <v>6927</v>
@@ -62448,7 +62448,7 @@
         <v>391</v>
       </c>
       <c r="D904" s="1" t="s">
-        <v>9390</v>
+        <v>9389</v>
       </c>
       <c r="E904" s="1" t="s">
         <v>7019</v>
@@ -62485,7 +62485,7 @@
         <v>1946</v>
       </c>
       <c r="D906" s="1" t="s">
-        <v>9484</v>
+        <v>9483</v>
       </c>
       <c r="E906" s="1" t="s">
         <v>2065</v>
@@ -62502,7 +62502,7 @@
         <v>15</v>
       </c>
       <c r="D907" s="1" t="s">
-        <v>9434</v>
+        <v>9433</v>
       </c>
       <c r="E907" s="1" t="s">
         <v>7170</v>
@@ -62687,7 +62687,7 @@
         <v>7117</v>
       </c>
       <c r="D917" s="1" t="s">
-        <v>9417</v>
+        <v>9416</v>
       </c>
       <c r="E917" s="1" t="s">
         <v>7118</v>
@@ -62704,7 +62704,7 @@
         <v>6868</v>
       </c>
       <c r="D918" s="1" t="s">
-        <v>9339</v>
+        <v>9338</v>
       </c>
       <c r="E918" s="1" t="s">
         <v>6869</v>
@@ -62724,7 +62724,7 @@
         <v>710</v>
       </c>
       <c r="D919" s="1" t="s">
-        <v>9347</v>
+        <v>9346</v>
       </c>
       <c r="E919" s="1" t="s">
         <v>6896</v>
@@ -62741,7 +62741,7 @@
         <v>445</v>
       </c>
       <c r="D920" s="1" t="s">
-        <v>9338</v>
+        <v>9337</v>
       </c>
       <c r="E920" s="1" t="s">
         <v>6865</v>
@@ -63523,7 +63523,7 @@
         <v>217</v>
       </c>
       <c r="D960" s="1" t="s">
-        <v>9313</v>
+        <v>9312</v>
       </c>
       <c r="E960" s="1" t="s">
         <v>6785</v>
@@ -63540,7 +63540,7 @@
         <v>5204</v>
       </c>
       <c r="D961" s="1" t="s">
-        <v>9314</v>
+        <v>9313</v>
       </c>
       <c r="E961" s="1" t="s">
         <v>6788</v>
@@ -63557,7 +63557,7 @@
         <v>15</v>
       </c>
       <c r="D962" s="1" t="s">
-        <v>9437</v>
+        <v>9436</v>
       </c>
       <c r="E962" s="1" t="s">
         <v>7179</v>
@@ -63574,7 +63574,7 @@
         <v>15</v>
       </c>
       <c r="D963" s="1" t="s">
-        <v>9438</v>
+        <v>9437</v>
       </c>
       <c r="E963" s="1" t="s">
         <v>7182</v>
@@ -63591,7 +63591,7 @@
         <v>15</v>
       </c>
       <c r="D964" s="1" t="s">
-        <v>9436</v>
+        <v>9435</v>
       </c>
       <c r="E964" s="1" t="s">
         <v>7176</v>
@@ -63668,7 +63668,7 @@
         <v>1950</v>
       </c>
       <c r="D968" s="1" t="s">
-        <v>9425</v>
+        <v>9424</v>
       </c>
       <c r="E968" s="1" t="s">
         <v>7136</v>
@@ -63742,7 +63742,7 @@
         <v>6062</v>
       </c>
       <c r="D972" s="1" t="s">
-        <v>9259</v>
+        <v>9258</v>
       </c>
       <c r="E972" s="1" t="s">
         <v>6078</v>
@@ -63899,7 +63899,7 @@
         <v>248</v>
       </c>
       <c r="D980" s="1" t="s">
-        <v>9410</v>
+        <v>9409</v>
       </c>
       <c r="E980" s="1" t="s">
         <v>7091</v>
@@ -63950,7 +63950,7 @@
         <v>7107</v>
       </c>
       <c r="D983" s="1" t="s">
-        <v>9414</v>
+        <v>9413</v>
       </c>
       <c r="E983" s="1" t="s">
         <v>7108</v>
@@ -63967,7 +63967,7 @@
         <v>7107</v>
       </c>
       <c r="D984" s="1" t="s">
-        <v>9416</v>
+        <v>9415</v>
       </c>
       <c r="E984" s="1" t="s">
         <v>7114</v>
@@ -63984,7 +63984,7 @@
         <v>7107</v>
       </c>
       <c r="D985" s="1" t="s">
-        <v>9415</v>
+        <v>9414</v>
       </c>
       <c r="E985" s="1" t="s">
         <v>7111</v>
@@ -64001,7 +64001,7 @@
         <v>391</v>
       </c>
       <c r="D986" t="s">
-        <v>9391</v>
+        <v>9390</v>
       </c>
       <c r="E986" t="s">
         <v>7034</v>
@@ -64018,7 +64018,7 @@
         <v>6372</v>
       </c>
       <c r="D987" t="s">
-        <v>9485</v>
+        <v>9484</v>
       </c>
       <c r="E987" t="s">
         <v>7037</v>
@@ -64035,13 +64035,13 @@
         <v>391</v>
       </c>
       <c r="D988" s="1" t="s">
-        <v>9486</v>
+        <v>9485</v>
       </c>
       <c r="E988" s="1" t="s">
+        <v>9391</v>
+      </c>
+      <c r="F988" t="s">
         <v>9392</v>
-      </c>
-      <c r="F988" t="s">
-        <v>9393</v>
       </c>
     </row>
     <row r="989" spans="1:6">
@@ -64300,7 +64300,7 @@
         <v>981</v>
       </c>
       <c r="D1002" s="1" t="s">
-        <v>9356</v>
+        <v>9355</v>
       </c>
       <c r="E1002" s="1" t="s">
         <v>6918</v>
@@ -64317,7 +64317,7 @@
         <v>271</v>
       </c>
       <c r="D1003" s="1" t="s">
-        <v>9334</v>
+        <v>9333</v>
       </c>
       <c r="E1003" s="1" t="s">
         <v>6853</v>
@@ -64334,7 +64334,7 @@
         <v>271</v>
       </c>
       <c r="D1004" s="1" t="s">
-        <v>9335</v>
+        <v>9334</v>
       </c>
       <c r="E1004" s="1" t="s">
         <v>6856</v>
@@ -64351,7 +64351,7 @@
         <v>1654</v>
       </c>
       <c r="D1005" s="1" t="s">
-        <v>9332</v>
+        <v>9331</v>
       </c>
       <c r="E1005" s="1" t="s">
         <v>6847</v>
@@ -64368,7 +64368,7 @@
         <v>1654</v>
       </c>
       <c r="D1006" s="1" t="s">
-        <v>9333</v>
+        <v>9332</v>
       </c>
       <c r="E1006" s="1" t="s">
         <v>6850</v>
@@ -64385,7 +64385,7 @@
         <v>271</v>
       </c>
       <c r="D1007" s="1" t="s">
-        <v>9336</v>
+        <v>9335</v>
       </c>
       <c r="E1007" s="1" t="s">
         <v>6859</v>
@@ -64490,7 +64490,7 @@
         <v>93</v>
       </c>
       <c r="D1013" t="s">
-        <v>9298</v>
+        <v>9297</v>
       </c>
       <c r="E1013" t="s">
         <v>6733</v>
@@ -64507,7 +64507,7 @@
         <v>395</v>
       </c>
       <c r="D1014" t="s">
-        <v>9297</v>
+        <v>9296</v>
       </c>
       <c r="E1014" t="s">
         <v>6730</v>
@@ -64524,7 +64524,7 @@
         <v>93</v>
       </c>
       <c r="D1015" t="s">
-        <v>9289</v>
+        <v>9288</v>
       </c>
       <c r="E1015" t="s">
         <v>6706</v>
@@ -64541,7 +64541,7 @@
         <v>93</v>
       </c>
       <c r="D1016" t="s">
-        <v>9293</v>
+        <v>9292</v>
       </c>
       <c r="E1016" t="s">
         <v>6718</v>
@@ -64558,7 +64558,7 @@
         <v>93</v>
       </c>
       <c r="D1017" t="s">
-        <v>9285</v>
+        <v>9284</v>
       </c>
       <c r="E1017" t="s">
         <v>6694</v>
@@ -64575,7 +64575,7 @@
         <v>93</v>
       </c>
       <c r="D1018" t="s">
-        <v>9290</v>
+        <v>9289</v>
       </c>
       <c r="E1018" t="s">
         <v>6709</v>
@@ -64592,7 +64592,7 @@
         <v>2912</v>
       </c>
       <c r="D1019" t="s">
-        <v>9294</v>
+        <v>9293</v>
       </c>
       <c r="E1019" t="s">
         <v>6721</v>
@@ -64609,7 +64609,7 @@
         <v>93</v>
       </c>
       <c r="D1020" t="s">
-        <v>9286</v>
+        <v>9285</v>
       </c>
       <c r="E1020" t="s">
         <v>6697</v>
@@ -64626,7 +64626,7 @@
         <v>93</v>
       </c>
       <c r="D1021" t="s">
-        <v>9292</v>
+        <v>9291</v>
       </c>
       <c r="E1021" t="s">
         <v>6715</v>
@@ -64643,7 +64643,7 @@
         <v>93</v>
       </c>
       <c r="D1022" t="s">
-        <v>9296</v>
+        <v>9295</v>
       </c>
       <c r="E1022" t="s">
         <v>6727</v>
@@ -64660,7 +64660,7 @@
         <v>93</v>
       </c>
       <c r="D1023" t="s">
-        <v>9288</v>
+        <v>9287</v>
       </c>
       <c r="E1023" t="s">
         <v>6703</v>
@@ -64677,7 +64677,7 @@
         <v>93</v>
       </c>
       <c r="D1024" t="s">
-        <v>9291</v>
+        <v>9290</v>
       </c>
       <c r="E1024" t="s">
         <v>6712</v>
@@ -64694,7 +64694,7 @@
         <v>93</v>
       </c>
       <c r="D1025" t="s">
-        <v>9295</v>
+        <v>9294</v>
       </c>
       <c r="E1025" t="s">
         <v>6724</v>
@@ -64711,7 +64711,7 @@
         <v>93</v>
       </c>
       <c r="D1026" t="s">
-        <v>9287</v>
+        <v>9286</v>
       </c>
       <c r="E1026" t="s">
         <v>6700</v>
@@ -65171,7 +65171,7 @@
         <v>6062</v>
       </c>
       <c r="D1049" s="1" t="s">
-        <v>9258</v>
+        <v>9257</v>
       </c>
       <c r="E1049" s="1" t="s">
         <v>6075</v>
@@ -65262,7 +65262,7 @@
         <v>248</v>
       </c>
       <c r="D1054" s="1" t="s">
-        <v>9389</v>
+        <v>9388</v>
       </c>
       <c r="E1054" s="1" t="s">
         <v>7014</v>
@@ -65553,7 +65553,7 @@
         <v>2795</v>
       </c>
       <c r="D1069" s="1" t="s">
-        <v>9487</v>
+        <v>9486</v>
       </c>
       <c r="E1069" s="1" t="s">
         <v>8629</v>
@@ -65593,7 +65593,7 @@
         <v>2569</v>
       </c>
       <c r="D1071" s="1" t="s">
-        <v>9488</v>
+        <v>9487</v>
       </c>
       <c r="E1071" s="1" t="s">
         <v>2612</v>
@@ -65747,7 +65747,7 @@
         <v>217</v>
       </c>
       <c r="D1079" s="4" t="s">
-        <v>9490</v>
+        <v>9489</v>
       </c>
       <c r="E1079" s="4" t="s">
         <v>6751</v>
@@ -65764,7 +65764,7 @@
         <v>93</v>
       </c>
       <c r="D1080" s="1" t="s">
-        <v>9489</v>
+        <v>9488</v>
       </c>
       <c r="E1080" s="1" t="s">
         <v>6742</v>
@@ -65781,7 +65781,7 @@
         <v>217</v>
       </c>
       <c r="D1081" t="s">
-        <v>9303</v>
+        <v>9302</v>
       </c>
       <c r="E1081" t="s">
         <v>6754</v>
@@ -65798,7 +65798,7 @@
         <v>217</v>
       </c>
       <c r="D1082" s="3" t="s">
-        <v>9304</v>
+        <v>9303</v>
       </c>
       <c r="E1082" s="3" t="s">
         <v>6757</v>
@@ -65815,7 +65815,7 @@
         <v>217</v>
       </c>
       <c r="D1083" t="s">
-        <v>9305</v>
+        <v>9304</v>
       </c>
       <c r="E1083" t="s">
         <v>6760</v>
@@ -65832,7 +65832,7 @@
         <v>217</v>
       </c>
       <c r="D1084" t="s">
-        <v>9306</v>
+        <v>9305</v>
       </c>
       <c r="E1084" t="s">
         <v>6763</v>
@@ -65849,7 +65849,7 @@
         <v>217</v>
       </c>
       <c r="D1085" t="s">
-        <v>9307</v>
+        <v>9306</v>
       </c>
       <c r="E1085" t="s">
         <v>6766</v>
@@ -65874,7 +65874,7 @@
         <v>217</v>
       </c>
       <c r="D1087" t="s">
-        <v>9308</v>
+        <v>9307</v>
       </c>
       <c r="E1087" t="s">
         <v>6770</v>
@@ -65911,7 +65911,7 @@
         <v>871</v>
       </c>
       <c r="D1089" s="1" t="s">
-        <v>9542</v>
+        <v>9541</v>
       </c>
       <c r="E1089" s="1" t="s">
         <v>972</v>
@@ -65928,7 +65928,7 @@
         <v>217</v>
       </c>
       <c r="D1090" s="1" t="s">
-        <v>9317</v>
+        <v>9316</v>
       </c>
       <c r="E1090" s="1" t="s">
         <v>6797</v>
@@ -66153,7 +66153,7 @@
         <v>1035</v>
       </c>
       <c r="D1102" s="1" t="s">
-        <v>9380</v>
+        <v>9379</v>
       </c>
       <c r="E1102" s="1" t="s">
         <v>6983</v>
@@ -66170,7 +66170,7 @@
         <v>1035</v>
       </c>
       <c r="D1103" s="1" t="s">
-        <v>9375</v>
+        <v>9374</v>
       </c>
       <c r="E1103" s="1" t="s">
         <v>6968</v>
@@ -66187,7 +66187,7 @@
         <v>1035</v>
       </c>
       <c r="D1104" s="1" t="s">
-        <v>9377</v>
+        <v>9376</v>
       </c>
       <c r="E1104" s="1" t="s">
         <v>6974</v>
@@ -66204,7 +66204,7 @@
         <v>1035</v>
       </c>
       <c r="D1105" s="1" t="s">
-        <v>9376</v>
+        <v>9375</v>
       </c>
       <c r="E1105" s="1" t="s">
         <v>6971</v>
@@ -66221,7 +66221,7 @@
         <v>1035</v>
       </c>
       <c r="D1106" s="1" t="s">
-        <v>9378</v>
+        <v>9377</v>
       </c>
       <c r="E1106" s="1" t="s">
         <v>6977</v>
@@ -66238,7 +66238,7 @@
         <v>1035</v>
       </c>
       <c r="D1107" s="1" t="s">
-        <v>9379</v>
+        <v>9378</v>
       </c>
       <c r="E1107" s="1" t="s">
         <v>6980</v>
@@ -66255,7 +66255,7 @@
         <v>1035</v>
       </c>
       <c r="D1108" s="1" t="s">
-        <v>9381</v>
+        <v>9380</v>
       </c>
       <c r="E1108" s="1" t="s">
         <v>6986</v>
@@ -66272,7 +66272,7 @@
         <v>1035</v>
       </c>
       <c r="D1109" s="1" t="s">
-        <v>9382</v>
+        <v>9381</v>
       </c>
       <c r="E1109" s="1" t="s">
         <v>6988</v>
@@ -66406,7 +66406,7 @@
         <v>2670</v>
       </c>
       <c r="D1116" t="s">
-        <v>9491</v>
+        <v>9490</v>
       </c>
       <c r="E1116" t="s">
         <v>2690</v>
@@ -66925,7 +66925,7 @@
         <v>93</v>
       </c>
       <c r="D1143" s="1" t="s">
-        <v>9300</v>
+        <v>9299</v>
       </c>
       <c r="E1143" s="1" t="s">
         <v>6739</v>
@@ -66945,7 +66945,7 @@
         <v>720</v>
       </c>
       <c r="D1144" s="1" t="s">
-        <v>9492</v>
+        <v>9491</v>
       </c>
       <c r="E1144" s="1" t="s">
         <v>825</v>
@@ -67042,7 +67042,7 @@
         <v>93</v>
       </c>
       <c r="D1149" s="1" t="s">
-        <v>9299</v>
+        <v>9298</v>
       </c>
       <c r="E1149" s="1" t="s">
         <v>6736</v>
@@ -67122,7 +67122,7 @@
         <v>1537</v>
       </c>
       <c r="D1153" s="1" t="s">
-        <v>9493</v>
+        <v>9492</v>
       </c>
       <c r="E1153" s="1" t="s">
         <v>8631</v>
@@ -67806,7 +67806,7 @@
         <v>885</v>
       </c>
       <c r="D1189" s="1" t="s">
-        <v>9365</v>
+        <v>9364</v>
       </c>
       <c r="E1189" s="1" t="s">
         <v>6936</v>
@@ -67823,7 +67823,7 @@
         <v>885</v>
       </c>
       <c r="D1190" s="1" t="s">
-        <v>9364</v>
+        <v>9363</v>
       </c>
       <c r="E1190" s="1" t="s">
         <v>6933</v>
@@ -68907,7 +68907,7 @@
         <v>3283</v>
       </c>
       <c r="D1246" s="1" t="s">
-        <v>9494</v>
+        <v>9493</v>
       </c>
       <c r="E1246" s="1" t="s">
         <v>3329</v>
@@ -69652,7 +69652,7 @@
         <v>2957</v>
       </c>
       <c r="D1284" s="1" t="s">
-        <v>9495</v>
+        <v>9494</v>
       </c>
       <c r="E1284" s="1" t="s">
         <v>3055</v>
@@ -69672,7 +69672,7 @@
         <v>2957</v>
       </c>
       <c r="D1285" s="1" t="s">
-        <v>9496</v>
+        <v>9495</v>
       </c>
       <c r="E1285" s="1" t="s">
         <v>8633</v>
@@ -69912,7 +69912,7 @@
         <v>2957</v>
       </c>
       <c r="D1297" s="1" t="s">
-        <v>9497</v>
+        <v>9496</v>
       </c>
       <c r="E1297" s="1" t="s">
         <v>3086</v>
@@ -70086,7 +70086,7 @@
         <v>2957</v>
       </c>
       <c r="D1306" s="1" t="s">
-        <v>9498</v>
+        <v>9497</v>
       </c>
       <c r="E1306" s="1" t="s">
         <v>3138</v>
@@ -71951,7 +71951,7 @@
         <v>42</v>
       </c>
       <c r="D1400" s="1" t="s">
-        <v>9331</v>
+        <v>9330</v>
       </c>
       <c r="E1400" s="1" t="s">
         <v>6844</v>
@@ -71968,7 +71968,7 @@
         <v>6840</v>
       </c>
       <c r="D1401" s="1" t="s">
-        <v>9330</v>
+        <v>9329</v>
       </c>
       <c r="E1401" s="1" t="s">
         <v>6841</v>
@@ -72028,7 +72028,7 @@
         <v>1892</v>
       </c>
       <c r="D1404" s="1" t="s">
-        <v>9499</v>
+        <v>9498</v>
       </c>
       <c r="E1404" s="1" t="s">
         <v>8623</v>
@@ -72065,7 +72065,7 @@
         <v>217</v>
       </c>
       <c r="D1406" s="1" t="s">
-        <v>9309</v>
+        <v>9308</v>
       </c>
       <c r="E1406" s="1" t="s">
         <v>6773</v>
@@ -72082,7 +72082,7 @@
         <v>217</v>
       </c>
       <c r="D1407" s="1" t="s">
-        <v>9312</v>
+        <v>9311</v>
       </c>
       <c r="E1407" s="1" t="s">
         <v>6782</v>
@@ -72142,7 +72142,7 @@
         <v>3445</v>
       </c>
       <c r="D1410" s="1" t="s">
-        <v>9500</v>
+        <v>9499</v>
       </c>
       <c r="E1410" s="1" t="s">
         <v>3489</v>
@@ -72162,7 +72162,7 @@
         <v>3445</v>
       </c>
       <c r="D1411" s="1" t="s">
-        <v>9501</v>
+        <v>9500</v>
       </c>
       <c r="E1411" s="1" t="s">
         <v>3492</v>
@@ -72182,7 +72182,7 @@
         <v>3445</v>
       </c>
       <c r="D1412" s="1" t="s">
-        <v>9502</v>
+        <v>9501</v>
       </c>
       <c r="E1412" s="1" t="s">
         <v>3496</v>
@@ -72573,7 +72573,7 @@
         <v>4283</v>
       </c>
       <c r="D1432" s="1" t="s">
-        <v>9503</v>
+        <v>9502</v>
       </c>
       <c r="E1432" s="1" t="s">
         <v>4295</v>
@@ -73023,7 +73023,7 @@
         <v>7</v>
       </c>
       <c r="D1456" s="1" t="s">
-        <v>9504</v>
+        <v>9503</v>
       </c>
       <c r="E1456" s="1" t="s">
         <v>5388</v>
@@ -73194,7 +73194,7 @@
         <v>2569</v>
       </c>
       <c r="D1465" s="1" t="s">
-        <v>9505</v>
+        <v>9504</v>
       </c>
       <c r="E1465" s="1" t="s">
         <v>2627</v>
@@ -73268,7 +73268,7 @@
         <v>2569</v>
       </c>
       <c r="D1469" s="1" t="s">
-        <v>9506</v>
+        <v>9505</v>
       </c>
       <c r="E1469" s="1" t="s">
         <v>2630</v>
@@ -73305,7 +73305,7 @@
         <v>2569</v>
       </c>
       <c r="D1471" s="1" t="s">
-        <v>9507</v>
+        <v>9506</v>
       </c>
       <c r="E1471" s="1" t="s">
         <v>2633</v>
@@ -73539,7 +73539,7 @@
         <v>2912</v>
       </c>
       <c r="D1483" s="1" t="s">
-        <v>9242</v>
+        <v>9241</v>
       </c>
       <c r="E1483" s="1" t="s">
         <v>6013</v>
@@ -74234,7 +74234,7 @@
         <v>681</v>
       </c>
       <c r="D1520" s="1" t="s">
-        <v>9420</v>
+        <v>9419</v>
       </c>
       <c r="E1520" s="1" t="s">
         <v>7127</v>
@@ -74467,7 +74467,7 @@
         <v>6998</v>
       </c>
       <c r="D1533" s="1" t="s">
-        <v>9386</v>
+        <v>9385</v>
       </c>
       <c r="E1533" s="1" t="s">
         <v>7002</v>
@@ -74504,7 +74504,7 @@
         <v>1407</v>
       </c>
       <c r="D1535" s="1" t="s">
-        <v>9403</v>
+        <v>9402</v>
       </c>
       <c r="E1535" s="1" t="s">
         <v>7070</v>
@@ -74709,13 +74709,13 @@
         <v>391</v>
       </c>
       <c r="D1546" s="1" t="s">
-        <v>9476</v>
+        <v>9475</v>
       </c>
       <c r="E1546" s="1" t="s">
         <v>7017</v>
       </c>
       <c r="F1546" s="1" t="s">
-        <v>9475</v>
+        <v>9474</v>
       </c>
     </row>
     <row r="1547" spans="1:6">
@@ -74786,7 +74786,7 @@
         <v>256</v>
       </c>
       <c r="D1550" s="1" t="s">
-        <v>9427</v>
+        <v>9426</v>
       </c>
       <c r="E1550" s="1" t="s">
         <v>7147</v>
@@ -74823,7 +74823,7 @@
         <v>4157</v>
       </c>
       <c r="D1552" s="1" t="s">
-        <v>9408</v>
+        <v>9407</v>
       </c>
       <c r="E1552" s="1" t="s">
         <v>7085</v>
@@ -76306,7 +76306,7 @@
         <v>3068</v>
       </c>
       <c r="D1629" s="1" t="s">
-        <v>9328</v>
+        <v>9327</v>
       </c>
       <c r="E1629" s="1" t="s">
         <v>6834</v>
@@ -76323,7 +76323,7 @@
         <v>61</v>
       </c>
       <c r="D1630" s="1" t="s">
-        <v>9363</v>
+        <v>9362</v>
       </c>
       <c r="E1630" s="1" t="s">
         <v>6930</v>
@@ -76704,7 +76704,7 @@
         <v>6998</v>
       </c>
       <c r="D1651" s="1" t="s">
-        <v>9385</v>
+        <v>9384</v>
       </c>
       <c r="E1651" s="1" t="s">
         <v>6999</v>
@@ -76721,7 +76721,7 @@
         <v>1986</v>
       </c>
       <c r="D1652" s="1" t="s">
-        <v>9337</v>
+        <v>9336</v>
       </c>
       <c r="E1652" s="1" t="s">
         <v>6862</v>
@@ -76775,7 +76775,7 @@
         <v>42</v>
       </c>
       <c r="D1655" s="1" t="s">
-        <v>9345</v>
+        <v>9344</v>
       </c>
       <c r="E1655" s="1" t="s">
         <v>6888</v>
@@ -77217,7 +77217,7 @@
         <v>974</v>
       </c>
       <c r="D1678" s="1" t="s">
-        <v>9344</v>
+        <v>9343</v>
       </c>
       <c r="E1678" s="1" t="s">
         <v>6885</v>
@@ -77314,7 +77314,7 @@
         <v>968</v>
       </c>
       <c r="D1683" s="1" t="s">
-        <v>9431</v>
+        <v>9430</v>
       </c>
       <c r="E1683" s="1" t="s">
         <v>7161</v>
@@ -77445,7 +77445,7 @@
         <v>1415</v>
       </c>
       <c r="D1690" s="1" t="s">
-        <v>9396</v>
+        <v>9395</v>
       </c>
       <c r="E1690" s="1" t="s">
         <v>7047</v>
@@ -77482,7 +77482,7 @@
         <v>7</v>
       </c>
       <c r="D1692" s="1" t="s">
-        <v>9088</v>
+        <v>9545</v>
       </c>
       <c r="E1692" s="1" t="s">
         <v>5536</v>
@@ -77519,7 +77519,7 @@
         <v>42</v>
       </c>
       <c r="D1694" s="1" t="s">
-        <v>9340</v>
+        <v>9339</v>
       </c>
       <c r="E1694" s="1" t="s">
         <v>6872</v>
@@ -77596,7 +77596,7 @@
         <v>7</v>
       </c>
       <c r="D1698" s="1" t="s">
-        <v>9089</v>
+        <v>9088</v>
       </c>
       <c r="E1698" s="1" t="s">
         <v>5539</v>
@@ -77647,7 +77647,7 @@
         <v>3009</v>
       </c>
       <c r="D1701" s="1" t="s">
-        <v>9405</v>
+        <v>9404</v>
       </c>
       <c r="E1701" s="1" t="s">
         <v>7076</v>
@@ -77664,7 +77664,7 @@
         <v>3068</v>
       </c>
       <c r="D1702" s="1" t="s">
-        <v>9329</v>
+        <v>9328</v>
       </c>
       <c r="E1702" s="1" t="s">
         <v>6838</v>
@@ -77701,7 +77701,7 @@
         <v>7</v>
       </c>
       <c r="D1704" s="1" t="s">
-        <v>9090</v>
+        <v>9089</v>
       </c>
       <c r="E1704" s="1" t="s">
         <v>5542</v>
@@ -77718,7 +77718,7 @@
         <v>7</v>
       </c>
       <c r="D1705" s="1" t="s">
-        <v>9091</v>
+        <v>9090</v>
       </c>
       <c r="E1705" s="1" t="s">
         <v>5545</v>
@@ -77735,7 +77735,7 @@
         <v>7</v>
       </c>
       <c r="D1706" s="1" t="s">
-        <v>9092</v>
+        <v>9091</v>
       </c>
       <c r="E1706" s="1" t="s">
         <v>5548</v>
@@ -77752,7 +77752,7 @@
         <v>271</v>
       </c>
       <c r="D1707" s="1" t="s">
-        <v>9093</v>
+        <v>9092</v>
       </c>
       <c r="E1707" s="1" t="s">
         <v>5551</v>
@@ -78509,7 +78509,7 @@
         <v>441</v>
       </c>
       <c r="D1745" s="1" t="s">
-        <v>9439</v>
+        <v>9438</v>
       </c>
       <c r="E1745" s="1" t="s">
         <v>7188</v>
@@ -78526,7 +78526,7 @@
         <v>462</v>
       </c>
       <c r="D1746" s="1" t="s">
-        <v>9406</v>
+        <v>9405</v>
       </c>
       <c r="E1746" s="1" t="s">
         <v>7079</v>
@@ -78543,7 +78543,7 @@
         <v>7</v>
       </c>
       <c r="D1747" s="1" t="s">
-        <v>9094</v>
+        <v>9093</v>
       </c>
       <c r="E1747" s="1" t="s">
         <v>5553</v>
@@ -78580,7 +78580,7 @@
         <v>1415</v>
       </c>
       <c r="D1749" s="1" t="s">
-        <v>9395</v>
+        <v>9394</v>
       </c>
       <c r="E1749" s="1" t="s">
         <v>7044</v>
@@ -78794,7 +78794,7 @@
         <v>7</v>
       </c>
       <c r="D1760" s="1" t="s">
-        <v>9095</v>
+        <v>9094</v>
       </c>
       <c r="E1760" s="1" t="s">
         <v>5556</v>
@@ -78828,7 +78828,7 @@
         <v>7</v>
       </c>
       <c r="D1762" s="1" t="s">
-        <v>9096</v>
+        <v>9095</v>
       </c>
       <c r="E1762" s="1" t="s">
         <v>5560</v>
@@ -78845,7 +78845,7 @@
         <v>7</v>
       </c>
       <c r="D1763" s="1" t="s">
-        <v>9097</v>
+        <v>9096</v>
       </c>
       <c r="E1763" s="1" t="s">
         <v>5564</v>
@@ -78919,7 +78919,7 @@
         <v>5131</v>
       </c>
       <c r="D1767" s="1" t="s">
-        <v>9430</v>
+        <v>9429</v>
       </c>
       <c r="E1767" s="1" t="s">
         <v>7158</v>
@@ -78959,7 +78959,7 @@
         <v>6062</v>
       </c>
       <c r="D1769" s="1" t="s">
-        <v>9532</v>
+        <v>9531</v>
       </c>
       <c r="E1769" s="1" t="s">
         <v>174</v>
@@ -78979,7 +78979,7 @@
         <v>6062</v>
       </c>
       <c r="D1770" s="1" t="s">
-        <v>9262</v>
+        <v>9261</v>
       </c>
       <c r="E1770" s="1" t="s">
         <v>6095</v>
@@ -79039,7 +79039,7 @@
         <v>6062</v>
       </c>
       <c r="D1773" s="1" t="s">
-        <v>9263</v>
+        <v>9262</v>
       </c>
       <c r="E1773" s="1" t="s">
         <v>6098</v>
@@ -79076,7 +79076,7 @@
         <v>1340</v>
       </c>
       <c r="D1775" s="1" t="s">
-        <v>9441</v>
+        <v>9440</v>
       </c>
       <c r="E1775" s="1" t="s">
         <v>7195</v>
@@ -79093,7 +79093,7 @@
         <v>6600</v>
       </c>
       <c r="D1776" s="1" t="s">
-        <v>9442</v>
+        <v>9441</v>
       </c>
       <c r="E1776" s="1" t="s">
         <v>7198</v>
@@ -79110,7 +79110,7 @@
         <v>6600</v>
       </c>
       <c r="D1777" s="1" t="s">
-        <v>9444</v>
+        <v>9443</v>
       </c>
       <c r="E1777" s="1" t="s">
         <v>7204</v>
@@ -79127,7 +79127,7 @@
         <v>6600</v>
       </c>
       <c r="D1778" s="1" t="s">
-        <v>9445</v>
+        <v>9444</v>
       </c>
       <c r="E1778" s="1" t="s">
         <v>7207</v>
@@ -79144,7 +79144,7 @@
         <v>1703</v>
       </c>
       <c r="D1779" s="1" t="s">
-        <v>9456</v>
+        <v>9455</v>
       </c>
       <c r="E1779" s="1" t="s">
         <v>7236</v>
@@ -79161,7 +79161,7 @@
         <v>1703</v>
       </c>
       <c r="D1780" s="4" t="s">
-        <v>9457</v>
+        <v>9456</v>
       </c>
       <c r="E1780" s="4" t="s">
         <v>7239</v>
@@ -79178,7 +79178,7 @@
         <v>6600</v>
       </c>
       <c r="D1781" s="1" t="s">
-        <v>9453</v>
+        <v>9452</v>
       </c>
       <c r="E1781" s="1" t="s">
         <v>7227</v>
@@ -79229,7 +79229,7 @@
         <v>6600</v>
       </c>
       <c r="D1784" s="1" t="s">
-        <v>9449</v>
+        <v>9448</v>
       </c>
       <c r="E1784" s="1" t="s">
         <v>7219</v>
@@ -79263,7 +79263,7 @@
         <v>6600</v>
       </c>
       <c r="D1786" s="1" t="s">
-        <v>9452</v>
+        <v>9451</v>
       </c>
       <c r="E1786" s="1" t="s">
         <v>7224</v>
@@ -79280,7 +79280,7 @@
         <v>6600</v>
       </c>
       <c r="D1787" s="1" t="s">
-        <v>9447</v>
+        <v>9446</v>
       </c>
       <c r="E1787" s="1" t="s">
         <v>7213</v>
@@ -79297,7 +79297,7 @@
         <v>6600</v>
       </c>
       <c r="D1788" s="1" t="s">
-        <v>9446</v>
+        <v>9445</v>
       </c>
       <c r="E1788" s="1" t="s">
         <v>7210</v>
@@ -79314,7 +79314,7 @@
         <v>6600</v>
       </c>
       <c r="D1789" s="1" t="s">
-        <v>9454</v>
+        <v>9453</v>
       </c>
       <c r="E1789" s="1" t="s">
         <v>7230</v>
@@ -79331,7 +79331,7 @@
         <v>1703</v>
       </c>
       <c r="D1790" s="1" t="s">
-        <v>9455</v>
+        <v>9454</v>
       </c>
       <c r="E1790" s="1" t="s">
         <v>7233</v>
@@ -79348,7 +79348,7 @@
         <v>6600</v>
       </c>
       <c r="D1791" s="1" t="s">
-        <v>9443</v>
+        <v>9442</v>
       </c>
       <c r="E1791" s="1" t="s">
         <v>7201</v>
@@ -79382,10 +79382,10 @@
         <v>6600</v>
       </c>
       <c r="D1793" s="1" t="s">
+        <v>9449</v>
+      </c>
+      <c r="E1793" s="1" t="s">
         <v>9450</v>
-      </c>
-      <c r="E1793" s="1" t="s">
-        <v>9451</v>
       </c>
       <c r="F1793" t="s">
         <v>7222</v>
@@ -79450,7 +79450,7 @@
         <v>7</v>
       </c>
       <c r="D1797" s="1" t="s">
-        <v>9098</v>
+        <v>9097</v>
       </c>
       <c r="E1797" s="1" t="s">
         <v>5566</v>
@@ -79467,7 +79467,7 @@
         <v>7</v>
       </c>
       <c r="D1798" s="1" t="s">
-        <v>9099</v>
+        <v>9098</v>
       </c>
       <c r="E1798" s="1" t="s">
         <v>5569</v>
@@ -79581,7 +79581,7 @@
         <v>7</v>
       </c>
       <c r="D1804" s="1" t="s">
-        <v>9100</v>
+        <v>9099</v>
       </c>
       <c r="E1804" s="1" t="s">
         <v>5572</v>
@@ -79598,7 +79598,7 @@
         <v>391</v>
       </c>
       <c r="D1805" s="1" t="s">
-        <v>9205</v>
+        <v>9204</v>
       </c>
       <c r="E1805" s="1" t="s">
         <v>7028</v>
@@ -79698,7 +79698,7 @@
         <v>3829</v>
       </c>
       <c r="D1810" s="1" t="s">
-        <v>9458</v>
+        <v>9457</v>
       </c>
       <c r="E1810" s="1" t="s">
         <v>4009</v>
@@ -79718,7 +79718,7 @@
         <v>3829</v>
       </c>
       <c r="D1811" s="1" t="s">
-        <v>9459</v>
+        <v>9458</v>
       </c>
       <c r="E1811" s="1" t="s">
         <v>4032</v>
@@ -79738,7 +79738,7 @@
         <v>3829</v>
       </c>
       <c r="D1812" s="1" t="s">
-        <v>9460</v>
+        <v>9459</v>
       </c>
       <c r="E1812" s="1" t="s">
         <v>4012</v>
@@ -79758,7 +79758,7 @@
         <v>3829</v>
       </c>
       <c r="D1813" s="1" t="s">
-        <v>9461</v>
+        <v>9460</v>
       </c>
       <c r="E1813" s="1" t="s">
         <v>4015</v>
@@ -79778,7 +79778,7 @@
         <v>3829</v>
       </c>
       <c r="D1814" s="1" t="s">
-        <v>9462</v>
+        <v>9461</v>
       </c>
       <c r="E1814" s="1" t="s">
         <v>4018</v>
@@ -79798,7 +79798,7 @@
         <v>3829</v>
       </c>
       <c r="D1815" s="1" t="s">
-        <v>9463</v>
+        <v>9462</v>
       </c>
       <c r="E1815" s="1" t="s">
         <v>4035</v>
@@ -79818,7 +79818,7 @@
         <v>3829</v>
       </c>
       <c r="D1816" s="1" t="s">
-        <v>9464</v>
+        <v>9463</v>
       </c>
       <c r="E1816" s="1" t="s">
         <v>4020</v>
@@ -79918,7 +79918,7 @@
         <v>6062</v>
       </c>
       <c r="D1821" s="1" t="s">
-        <v>9260</v>
+        <v>9259</v>
       </c>
       <c r="E1821" s="1" t="s">
         <v>6081</v>
@@ -80152,7 +80152,7 @@
         <v>5595</v>
       </c>
       <c r="D1833" s="1" t="s">
-        <v>9384</v>
+        <v>9383</v>
       </c>
       <c r="E1833" s="1" t="s">
         <v>6995</v>
@@ -80409,7 +80409,7 @@
         <v>7</v>
       </c>
       <c r="D1846" t="s">
-        <v>9101</v>
+        <v>9100</v>
       </c>
       <c r="E1846" t="s">
         <v>5576</v>
@@ -80486,7 +80486,7 @@
         <v>4241</v>
       </c>
       <c r="D1850" s="1" t="s">
-        <v>9533</v>
+        <v>9532</v>
       </c>
       <c r="E1850" s="1" t="s">
         <v>174</v>
@@ -80503,7 +80503,7 @@
         <v>7</v>
       </c>
       <c r="D1851" s="1" t="s">
-        <v>9102</v>
+        <v>9101</v>
       </c>
       <c r="E1851" s="1" t="s">
         <v>5582</v>
@@ -80580,7 +80580,7 @@
         <v>2161</v>
       </c>
       <c r="D1855" s="1" t="s">
-        <v>9244</v>
+        <v>9243</v>
       </c>
       <c r="E1855" s="1" t="s">
         <v>6019</v>
@@ -80671,7 +80671,7 @@
         <v>7</v>
       </c>
       <c r="D1860" s="1" t="s">
-        <v>9104</v>
+        <v>9103</v>
       </c>
       <c r="E1860" s="1" t="s">
         <v>5593</v>
@@ -80717,7 +80717,7 @@
         <v>174</v>
       </c>
       <c r="F1862" s="1" t="s">
-        <v>9534</v>
+        <v>9533</v>
       </c>
     </row>
     <row r="1863" spans="1:6">
@@ -80808,7 +80808,7 @@
         <v>217</v>
       </c>
       <c r="D1867" s="1" t="s">
-        <v>9301</v>
+        <v>9300</v>
       </c>
       <c r="E1867" s="1" t="s">
         <v>6745</v>
@@ -80825,7 +80825,7 @@
         <v>217</v>
       </c>
       <c r="D1868" s="1" t="s">
-        <v>9302</v>
+        <v>9301</v>
       </c>
       <c r="E1868" s="1" t="s">
         <v>6748</v>
@@ -81002,7 +81002,7 @@
         <v>5595</v>
       </c>
       <c r="D1877" s="1" t="s">
-        <v>9105</v>
+        <v>9104</v>
       </c>
       <c r="E1877" s="1" t="s">
         <v>5596</v>
@@ -81019,7 +81019,7 @@
         <v>4326</v>
       </c>
       <c r="D1878" s="1" t="s">
-        <v>9106</v>
+        <v>9105</v>
       </c>
       <c r="E1878" s="1" t="s">
         <v>5600</v>
@@ -81156,7 +81156,7 @@
         <v>7</v>
       </c>
       <c r="D1885" s="1" t="s">
-        <v>9107</v>
+        <v>9106</v>
       </c>
       <c r="E1885" s="1" t="s">
         <v>5602</v>
@@ -81173,7 +81173,7 @@
         <v>7</v>
       </c>
       <c r="D1886" s="1" t="s">
-        <v>9108</v>
+        <v>9107</v>
       </c>
       <c r="E1886" s="1" t="s">
         <v>5604</v>
@@ -81227,7 +81227,7 @@
         <v>7</v>
       </c>
       <c r="D1889" s="1" t="s">
-        <v>9109</v>
+        <v>9108</v>
       </c>
       <c r="E1889" s="1" t="s">
         <v>5609</v>
@@ -81264,7 +81264,7 @@
         <v>7</v>
       </c>
       <c r="D1891" s="1" t="s">
-        <v>9110</v>
+        <v>9109</v>
       </c>
       <c r="E1891" s="1" t="s">
         <v>5611</v>
@@ -81281,7 +81281,7 @@
         <v>7</v>
       </c>
       <c r="D1892" s="1" t="s">
-        <v>9111</v>
+        <v>9110</v>
       </c>
       <c r="E1892" s="1" t="s">
         <v>5613</v>
@@ -81475,7 +81475,7 @@
         <v>1247</v>
       </c>
       <c r="D1902" s="1" t="s">
-        <v>9397</v>
+        <v>9396</v>
       </c>
       <c r="E1902" s="1" t="s">
         <v>7052</v>
@@ -81589,7 +81589,7 @@
         <v>7</v>
       </c>
       <c r="D1908" s="1" t="s">
-        <v>9112</v>
+        <v>9111</v>
       </c>
       <c r="E1908" s="1" t="s">
         <v>5619</v>
@@ -81686,7 +81686,7 @@
         <v>7</v>
       </c>
       <c r="D1913" s="1" t="s">
-        <v>9113</v>
+        <v>9112</v>
       </c>
       <c r="E1913" s="1" t="s">
         <v>5622</v>
@@ -81743,7 +81743,7 @@
         <v>7</v>
       </c>
       <c r="D1916" s="1" t="s">
-        <v>9114</v>
+        <v>9113</v>
       </c>
       <c r="E1916" s="1" t="s">
         <v>5625</v>
@@ -81860,7 +81860,7 @@
         <v>1703</v>
       </c>
       <c r="D1922" s="4" t="s">
-        <v>9116</v>
+        <v>9115</v>
       </c>
       <c r="E1922" s="4" t="s">
         <v>5631</v>
@@ -81877,7 +81877,7 @@
         <v>1703</v>
       </c>
       <c r="D1923" s="4" t="s">
-        <v>9115</v>
+        <v>9114</v>
       </c>
       <c r="E1923" s="4" t="s">
         <v>5628</v>
@@ -81914,7 +81914,7 @@
         <v>7</v>
       </c>
       <c r="D1925" s="4" t="s">
-        <v>9117</v>
+        <v>9116</v>
       </c>
       <c r="E1925" s="4" t="s">
         <v>5634</v>
@@ -81931,7 +81931,7 @@
         <v>7</v>
       </c>
       <c r="D1926" s="1" t="s">
-        <v>9118</v>
+        <v>9117</v>
       </c>
       <c r="E1926" s="1" t="s">
         <v>5637</v>
@@ -81948,7 +81948,7 @@
         <v>7</v>
       </c>
       <c r="D1927" s="1" t="s">
-        <v>9119</v>
+        <v>9118</v>
       </c>
       <c r="E1927" s="1" t="s">
         <v>5640</v>
@@ -82025,7 +82025,7 @@
         <v>7</v>
       </c>
       <c r="D1931" s="1" t="s">
-        <v>9119</v>
+        <v>9118</v>
       </c>
       <c r="E1931" s="1" t="s">
         <v>5640</v>
@@ -82082,7 +82082,7 @@
         <v>7</v>
       </c>
       <c r="D1934" s="1" t="s">
-        <v>9120</v>
+        <v>9119</v>
       </c>
       <c r="E1934" s="1" t="s">
         <v>5644</v>
@@ -82139,7 +82139,7 @@
         <v>7</v>
       </c>
       <c r="D1937" s="1" t="s">
-        <v>9121</v>
+        <v>9120</v>
       </c>
       <c r="E1937" s="1" t="s">
         <v>5647</v>
@@ -82176,7 +82176,7 @@
         <v>7</v>
       </c>
       <c r="D1939" s="1" t="s">
-        <v>9123</v>
+        <v>9122</v>
       </c>
       <c r="E1939" s="1" t="s">
         <v>5653</v>
@@ -82213,7 +82213,7 @@
         <v>7</v>
       </c>
       <c r="D1941" s="1" t="s">
-        <v>9124</v>
+        <v>9123</v>
       </c>
       <c r="E1941" s="1" t="s">
         <v>5656</v>
@@ -82230,7 +82230,7 @@
         <v>7</v>
       </c>
       <c r="D1942" s="1" t="s">
-        <v>9125</v>
+        <v>9124</v>
       </c>
       <c r="E1942" s="1" t="s">
         <v>5659</v>
@@ -82721,7 +82721,7 @@
         <v>7</v>
       </c>
       <c r="D1967" s="1" t="s">
-        <v>9126</v>
+        <v>9125</v>
       </c>
       <c r="E1967" s="1" t="s">
         <v>5662</v>
@@ -82738,7 +82738,7 @@
         <v>7</v>
       </c>
       <c r="D1968" s="1" t="s">
-        <v>9127</v>
+        <v>9126</v>
       </c>
       <c r="E1968" s="1" t="s">
         <v>5665</v>
@@ -82755,7 +82755,7 @@
         <v>7</v>
       </c>
       <c r="D1969" s="1" t="s">
-        <v>9128</v>
+        <v>9127</v>
       </c>
       <c r="E1969" s="1" t="s">
         <v>5668</v>
@@ -82772,7 +82772,7 @@
         <v>7</v>
       </c>
       <c r="D1970" s="1" t="s">
-        <v>9129</v>
+        <v>9128</v>
       </c>
       <c r="E1970" s="1" t="s">
         <v>5671</v>
@@ -82789,7 +82789,7 @@
         <v>7</v>
       </c>
       <c r="D1971" s="1" t="s">
-        <v>9130</v>
+        <v>9129</v>
       </c>
       <c r="E1971" s="1" t="s">
         <v>5674</v>
@@ -82806,7 +82806,7 @@
         <v>7</v>
       </c>
       <c r="D1972" s="1" t="s">
-        <v>9131</v>
+        <v>9130</v>
       </c>
       <c r="E1972" s="1" t="s">
         <v>5677</v>
@@ -82823,7 +82823,7 @@
         <v>7</v>
       </c>
       <c r="D1973" s="1" t="s">
-        <v>9132</v>
+        <v>9131</v>
       </c>
       <c r="E1973" s="1" t="s">
         <v>5680</v>
@@ -82840,7 +82840,7 @@
         <v>7</v>
       </c>
       <c r="D1974" s="1" t="s">
-        <v>9133</v>
+        <v>9132</v>
       </c>
       <c r="E1974" s="1" t="s">
         <v>5683</v>
@@ -82857,7 +82857,7 @@
         <v>7</v>
       </c>
       <c r="D1975" s="1" t="s">
-        <v>9134</v>
+        <v>9133</v>
       </c>
       <c r="E1975" s="1" t="s">
         <v>5686</v>
@@ -82891,7 +82891,7 @@
         <v>7</v>
       </c>
       <c r="D1977" s="1" t="s">
-        <v>9135</v>
+        <v>9134</v>
       </c>
       <c r="E1977" s="1" t="s">
         <v>5690</v>
@@ -82988,7 +82988,7 @@
         <v>7</v>
       </c>
       <c r="D1982" s="1" t="s">
-        <v>9136</v>
+        <v>9135</v>
       </c>
       <c r="E1982" s="1" t="s">
         <v>5692</v>
@@ -83005,7 +83005,7 @@
         <v>7</v>
       </c>
       <c r="D1983" s="1" t="s">
-        <v>9137</v>
+        <v>9136</v>
       </c>
       <c r="E1983" s="1" t="s">
         <v>5696</v>
@@ -83202,7 +83202,7 @@
         <v>7</v>
       </c>
       <c r="D1993" s="1" t="s">
-        <v>9138</v>
+        <v>9137</v>
       </c>
       <c r="E1993" s="1" t="s">
         <v>5698</v>
@@ -83242,7 +83242,7 @@
         <v>2807</v>
       </c>
       <c r="D1995" s="1" t="s">
-        <v>9465</v>
+        <v>9464</v>
       </c>
       <c r="E1995" s="1" t="s">
         <v>4111</v>
@@ -83259,7 +83259,7 @@
         <v>7</v>
       </c>
       <c r="D1996" s="1" t="s">
-        <v>9139</v>
+        <v>9138</v>
       </c>
       <c r="E1996" s="1" t="s">
         <v>5701</v>
@@ -83276,7 +83276,7 @@
         <v>7</v>
       </c>
       <c r="D1997" s="1" t="s">
-        <v>9140</v>
+        <v>9139</v>
       </c>
       <c r="E1997" s="1" t="s">
         <v>5704</v>
@@ -83293,7 +83293,7 @@
         <v>7</v>
       </c>
       <c r="D1998" s="1" t="s">
-        <v>9141</v>
+        <v>9140</v>
       </c>
       <c r="E1998" s="1" t="s">
         <v>5707</v>
@@ -83350,7 +83350,7 @@
         <v>7</v>
       </c>
       <c r="D2001" s="1" t="s">
-        <v>9142</v>
+        <v>9141</v>
       </c>
       <c r="E2001" s="1" t="s">
         <v>5710</v>
@@ -83427,7 +83427,7 @@
         <v>7</v>
       </c>
       <c r="D2005" s="1" t="s">
-        <v>9143</v>
+        <v>9142</v>
       </c>
       <c r="E2005" s="1" t="s">
         <v>5713</v>
@@ -83504,7 +83504,7 @@
         <v>7</v>
       </c>
       <c r="D2009" s="1" t="s">
-        <v>9144</v>
+        <v>9143</v>
       </c>
       <c r="E2009" s="1" t="s">
         <v>5716</v>
@@ -83664,7 +83664,7 @@
         <v>710</v>
       </c>
       <c r="D2017" s="1" t="s">
-        <v>9243</v>
+        <v>9242</v>
       </c>
       <c r="E2017" s="1" t="s">
         <v>6016</v>
@@ -83704,7 +83704,7 @@
         <v>6062</v>
       </c>
       <c r="D2019" s="1" t="s">
-        <v>9261</v>
+        <v>9260</v>
       </c>
       <c r="E2019" s="1" t="s">
         <v>6088</v>
@@ -83841,7 +83841,7 @@
         <v>137</v>
       </c>
       <c r="D2026" s="1" t="s">
-        <v>9466</v>
+        <v>9465</v>
       </c>
       <c r="E2026" s="1" t="s">
         <v>6486</v>
@@ -83878,7 +83878,7 @@
         <v>7</v>
       </c>
       <c r="D2028" s="1" t="s">
-        <v>9145</v>
+        <v>9144</v>
       </c>
       <c r="E2028" s="1" t="s">
         <v>5719</v>
@@ -83915,7 +83915,7 @@
         <v>7</v>
       </c>
       <c r="D2030" s="1" t="s">
-        <v>9146</v>
+        <v>9145</v>
       </c>
       <c r="E2030" s="1" t="s">
         <v>5722</v>
@@ -83983,7 +83983,7 @@
         <v>7</v>
       </c>
       <c r="D2034" s="1" t="s">
-        <v>9147</v>
+        <v>9146</v>
       </c>
       <c r="E2034" s="1" t="s">
         <v>5726</v>
@@ -84060,7 +84060,7 @@
         <v>7</v>
       </c>
       <c r="D2038" s="1" t="s">
-        <v>9148</v>
+        <v>9147</v>
       </c>
       <c r="E2038" s="1" t="s">
         <v>5728</v>
@@ -84077,7 +84077,7 @@
         <v>7</v>
       </c>
       <c r="D2039" s="1" t="s">
-        <v>9149</v>
+        <v>9148</v>
       </c>
       <c r="E2039" s="1" t="s">
         <v>5731</v>
@@ -84177,13 +84177,13 @@
         <v>6898</v>
       </c>
       <c r="D2044" s="1" t="s">
-        <v>9508</v>
+        <v>9507</v>
       </c>
       <c r="E2044" s="1" t="s">
-        <v>9355</v>
+        <v>9354</v>
       </c>
       <c r="F2044" s="1" t="s">
-        <v>9355</v>
+        <v>9354</v>
       </c>
     </row>
     <row r="2045" spans="1:6">
@@ -84197,7 +84197,7 @@
         <v>6898</v>
       </c>
       <c r="D2045" s="1" t="s">
-        <v>9348</v>
+        <v>9347</v>
       </c>
       <c r="E2045" s="1" t="s">
         <v>6899</v>
@@ -84217,7 +84217,7 @@
         <v>6898</v>
       </c>
       <c r="D2046" s="1" t="s">
-        <v>9351</v>
+        <v>9350</v>
       </c>
       <c r="E2046" s="1" t="s">
         <v>6910</v>
@@ -84254,7 +84254,7 @@
         <v>6898</v>
       </c>
       <c r="D2048" s="1" t="s">
-        <v>9350</v>
+        <v>9349</v>
       </c>
       <c r="E2048" s="1" t="s">
         <v>6905</v>
@@ -84274,13 +84274,13 @@
         <v>6898</v>
       </c>
       <c r="D2049" s="1" t="s">
-        <v>9509</v>
+        <v>9508</v>
       </c>
       <c r="E2049" s="1" t="s">
+        <v>9352</v>
+      </c>
+      <c r="F2049" t="s">
         <v>9353</v>
-      </c>
-      <c r="F2049" t="s">
-        <v>9354</v>
       </c>
     </row>
     <row r="2050" spans="1:6">
@@ -84314,7 +84314,7 @@
         <v>6898</v>
       </c>
       <c r="D2051" s="1" t="s">
-        <v>9349</v>
+        <v>9348</v>
       </c>
       <c r="E2051" s="1" t="s">
         <v>6902</v>
@@ -84334,7 +84334,7 @@
         <v>6898</v>
       </c>
       <c r="D2052" s="1" t="s">
-        <v>9352</v>
+        <v>9351</v>
       </c>
       <c r="E2052" s="1" t="s">
         <v>6913</v>
@@ -84371,7 +84371,7 @@
         <v>15</v>
       </c>
       <c r="D2054" s="1" t="s">
-        <v>9432</v>
+        <v>9431</v>
       </c>
       <c r="E2054" s="1" t="s">
         <v>7164</v>
@@ -84388,7 +84388,7 @@
         <v>15</v>
       </c>
       <c r="D2055" s="1" t="s">
-        <v>9433</v>
+        <v>9432</v>
       </c>
       <c r="E2055" s="1" t="s">
         <v>7167</v>
@@ -84465,7 +84465,7 @@
         <v>7</v>
       </c>
       <c r="D2059" s="1" t="s">
-        <v>9150</v>
+        <v>9149</v>
       </c>
       <c r="E2059" s="1" t="s">
         <v>5734</v>
@@ -84662,7 +84662,7 @@
         <v>7</v>
       </c>
       <c r="D2069" s="1" t="s">
-        <v>9151</v>
+        <v>9150</v>
       </c>
       <c r="E2069" s="1" t="s">
         <v>5737</v>
@@ -84999,7 +84999,7 @@
         <v>6924</v>
       </c>
       <c r="D2086" s="1" t="s">
-        <v>9409</v>
+        <v>9408</v>
       </c>
       <c r="E2086" s="1" t="s">
         <v>7088</v>
@@ -85093,7 +85093,7 @@
         <v>93</v>
       </c>
       <c r="D2091" s="1" t="s">
-        <v>9280</v>
+        <v>9279</v>
       </c>
       <c r="E2091" s="1" t="s">
         <v>6676</v>
@@ -85110,7 +85110,7 @@
         <v>3171</v>
       </c>
       <c r="D2092" s="1" t="s">
-        <v>9278</v>
+        <v>9277</v>
       </c>
       <c r="E2092" s="1" t="s">
         <v>6671</v>
@@ -85127,10 +85127,10 @@
         <v>93</v>
       </c>
       <c r="D2093" s="1" t="s">
-        <v>9279</v>
+        <v>9278</v>
       </c>
       <c r="E2093" s="1" t="s">
-        <v>9510</v>
+        <v>9509</v>
       </c>
       <c r="F2093" t="s">
         <v>6674</v>
@@ -85144,7 +85144,7 @@
         <v>3171</v>
       </c>
       <c r="D2094" s="1" t="s">
-        <v>9277</v>
+        <v>9276</v>
       </c>
       <c r="E2094" s="1" t="s">
         <v>6668</v>
@@ -85161,7 +85161,7 @@
         <v>3171</v>
       </c>
       <c r="D2095" s="1" t="s">
-        <v>9275</v>
+        <v>9274</v>
       </c>
       <c r="E2095" s="1" t="s">
         <v>6662</v>
@@ -85178,7 +85178,7 @@
         <v>3171</v>
       </c>
       <c r="D2096" s="1" t="s">
-        <v>9276</v>
+        <v>9275</v>
       </c>
       <c r="E2096" s="1" t="s">
         <v>6665</v>
@@ -85235,7 +85235,7 @@
         <v>117</v>
       </c>
       <c r="D2099" s="1" t="s">
-        <v>9511</v>
+        <v>9510</v>
       </c>
       <c r="E2099" s="1" t="s">
         <v>6329</v>
@@ -85569,7 +85569,7 @@
         <v>7</v>
       </c>
       <c r="D2116" s="1" t="s">
-        <v>9152</v>
+        <v>9151</v>
       </c>
       <c r="E2116" s="1" t="s">
         <v>5741</v>
@@ -85586,7 +85586,7 @@
         <v>7</v>
       </c>
       <c r="D2117" s="1" t="s">
-        <v>9153</v>
+        <v>9152</v>
       </c>
       <c r="E2117" s="1" t="s">
         <v>5744</v>
@@ -85603,7 +85603,7 @@
         <v>7</v>
       </c>
       <c r="D2118" s="1" t="s">
-        <v>9154</v>
+        <v>9153</v>
       </c>
       <c r="E2118" s="1" t="s">
         <v>5747</v>
@@ -85620,7 +85620,7 @@
         <v>7</v>
       </c>
       <c r="D2119" s="1" t="s">
-        <v>9155</v>
+        <v>9154</v>
       </c>
       <c r="E2119" s="1" t="s">
         <v>5750</v>
@@ -85637,7 +85637,7 @@
         <v>7</v>
       </c>
       <c r="D2120" s="1" t="s">
-        <v>9156</v>
+        <v>9155</v>
       </c>
       <c r="E2120" s="1" t="s">
         <v>5753</v>
@@ -85654,7 +85654,7 @@
         <v>7</v>
       </c>
       <c r="D2121" s="1" t="s">
-        <v>9157</v>
+        <v>9156</v>
       </c>
       <c r="E2121" s="1" t="s">
         <v>5756</v>
@@ -85671,7 +85671,7 @@
         <v>7</v>
       </c>
       <c r="D2122" s="1" t="s">
-        <v>9158</v>
+        <v>9157</v>
       </c>
       <c r="E2122" s="1" t="s">
         <v>5759</v>
@@ -85788,7 +85788,7 @@
         <v>7</v>
       </c>
       <c r="D2128" s="1" t="s">
-        <v>9159</v>
+        <v>9158</v>
       </c>
       <c r="E2128" s="1" t="s">
         <v>5762</v>
@@ -85825,7 +85825,7 @@
         <v>7</v>
       </c>
       <c r="D2130" s="1" t="s">
-        <v>9160</v>
+        <v>9159</v>
       </c>
       <c r="E2130" s="1" t="s">
         <v>5765</v>
@@ -85842,7 +85842,7 @@
         <v>6610</v>
       </c>
       <c r="D2131" s="1" t="s">
-        <v>9512</v>
+        <v>9511</v>
       </c>
       <c r="E2131" s="1" t="s">
         <v>6614</v>
@@ -85899,7 +85899,7 @@
         <v>217</v>
       </c>
       <c r="D2134" s="1" t="s">
-        <v>9315</v>
+        <v>9314</v>
       </c>
       <c r="E2134" s="1" t="s">
         <v>6791</v>
@@ -86076,7 +86076,7 @@
         <v>7</v>
       </c>
       <c r="D2143" s="1" t="s">
-        <v>9161</v>
+        <v>9160</v>
       </c>
       <c r="E2143" s="1" t="s">
         <v>5768</v>
@@ -86173,7 +86173,7 @@
         <v>7</v>
       </c>
       <c r="D2148" s="1" t="s">
-        <v>9162</v>
+        <v>9161</v>
       </c>
       <c r="E2148" s="1" t="s">
         <v>5772</v>
@@ -86210,7 +86210,7 @@
         <v>7</v>
       </c>
       <c r="D2150" s="1" t="s">
-        <v>9163</v>
+        <v>9162</v>
       </c>
       <c r="E2150" s="1" t="s">
         <v>5773</v>
@@ -86287,7 +86287,7 @@
         <v>7</v>
       </c>
       <c r="D2154" s="1" t="s">
-        <v>9164</v>
+        <v>9163</v>
       </c>
       <c r="E2154" s="1" t="s">
         <v>5775</v>
@@ -86361,7 +86361,7 @@
         <v>7</v>
       </c>
       <c r="D2158" s="1" t="s">
-        <v>9165</v>
+        <v>9164</v>
       </c>
       <c r="E2158" s="1" t="s">
         <v>5781</v>
@@ -86378,7 +86378,7 @@
         <v>6804</v>
       </c>
       <c r="D2159" s="1" t="s">
-        <v>9324</v>
+        <v>9323</v>
       </c>
       <c r="E2159" s="1" t="s">
         <v>6822</v>
@@ -86395,7 +86395,7 @@
         <v>6804</v>
       </c>
       <c r="D2160" s="1" t="s">
-        <v>9320</v>
+        <v>9319</v>
       </c>
       <c r="E2160" s="1" t="s">
         <v>6808</v>
@@ -86412,7 +86412,7 @@
         <v>6804</v>
       </c>
       <c r="D2161" s="1" t="s">
-        <v>9319</v>
+        <v>9318</v>
       </c>
       <c r="E2161" s="1" t="s">
         <v>6805</v>
@@ -86429,7 +86429,7 @@
         <v>6804</v>
       </c>
       <c r="D2162" s="1" t="s">
-        <v>9323</v>
+        <v>9322</v>
       </c>
       <c r="E2162" s="1" t="s">
         <v>6817</v>
@@ -86463,7 +86463,7 @@
         <v>6804</v>
       </c>
       <c r="D2164" s="1" t="s">
-        <v>9322</v>
+        <v>9321</v>
       </c>
       <c r="E2164" s="1" t="s">
         <v>6814</v>
@@ -86480,7 +86480,7 @@
         <v>6804</v>
       </c>
       <c r="D2165" s="1" t="s">
-        <v>9321</v>
+        <v>9320</v>
       </c>
       <c r="E2165" s="1" t="s">
         <v>6811</v>
@@ -86537,13 +86537,13 @@
         <v>7</v>
       </c>
       <c r="D2168" s="1" t="s">
-        <v>9513</v>
+        <v>9512</v>
       </c>
       <c r="E2168" s="1" t="s">
+        <v>9165</v>
+      </c>
+      <c r="F2168" t="s">
         <v>9166</v>
-      </c>
-      <c r="F2168" t="s">
-        <v>9167</v>
       </c>
     </row>
     <row r="2169" spans="1:6">
@@ -86554,13 +86554,13 @@
         <v>7</v>
       </c>
       <c r="D2169" s="1" t="s">
-        <v>9514</v>
+        <v>9513</v>
       </c>
       <c r="E2169" s="1" t="s">
+        <v>9167</v>
+      </c>
+      <c r="F2169" s="1" t="s">
         <v>9168</v>
-      </c>
-      <c r="F2169" s="1" t="s">
-        <v>9169</v>
       </c>
     </row>
     <row r="2170" spans="1:6">
@@ -86571,13 +86571,13 @@
         <v>7</v>
       </c>
       <c r="D2170" s="1" t="s">
-        <v>9515</v>
+        <v>9514</v>
       </c>
       <c r="E2170" s="1" t="s">
+        <v>9169</v>
+      </c>
+      <c r="F2170" s="1" t="s">
         <v>9170</v>
-      </c>
-      <c r="F2170" s="1" t="s">
-        <v>9171</v>
       </c>
     </row>
     <row r="2171" spans="1:6">
@@ -86588,13 +86588,13 @@
         <v>7</v>
       </c>
       <c r="D2171" s="1" t="s">
+        <v>9171</v>
+      </c>
+      <c r="E2171" s="1" t="s">
         <v>9172</v>
       </c>
-      <c r="E2171" s="1" t="s">
+      <c r="F2171" s="1" t="s">
         <v>9173</v>
-      </c>
-      <c r="F2171" s="1" t="s">
-        <v>9174</v>
       </c>
     </row>
     <row r="2172" spans="1:6">
@@ -86622,7 +86622,7 @@
         <v>7</v>
       </c>
       <c r="D2173" s="1" t="s">
-        <v>9178</v>
+        <v>9177</v>
       </c>
       <c r="E2173" s="1" t="s">
         <v>5802</v>
@@ -86639,7 +86639,7 @@
         <v>7</v>
       </c>
       <c r="D2174" s="1" t="s">
-        <v>9175</v>
+        <v>9174</v>
       </c>
       <c r="E2174" s="1" t="s">
         <v>5791</v>
@@ -86673,7 +86673,7 @@
         <v>7</v>
       </c>
       <c r="D2176" s="1" t="s">
-        <v>9176</v>
+        <v>9175</v>
       </c>
       <c r="E2176" s="1" t="s">
         <v>5796</v>
@@ -86690,7 +86690,7 @@
         <v>7</v>
       </c>
       <c r="D2177" s="1" t="s">
-        <v>9177</v>
+        <v>9176</v>
       </c>
       <c r="E2177" s="1" t="s">
         <v>5799</v>
@@ -86861,7 +86861,7 @@
         <v>7</v>
       </c>
       <c r="D2186" s="1" t="s">
-        <v>9179</v>
+        <v>9178</v>
       </c>
       <c r="E2186" s="1" t="s">
         <v>5809</v>
@@ -87018,7 +87018,7 @@
         <v>7</v>
       </c>
       <c r="D2194" s="1" t="s">
-        <v>9180</v>
+        <v>9179</v>
       </c>
       <c r="E2194" s="1" t="s">
         <v>5812</v>
@@ -87035,7 +87035,7 @@
         <v>7</v>
       </c>
       <c r="D2195" s="1" t="s">
-        <v>9181</v>
+        <v>9180</v>
       </c>
       <c r="E2195" s="1" t="s">
         <v>5815</v>
@@ -87129,7 +87129,7 @@
         <v>7</v>
       </c>
       <c r="D2200" s="1" t="s">
-        <v>9182</v>
+        <v>9181</v>
       </c>
       <c r="E2200" s="1" t="s">
         <v>5818</v>
@@ -87186,7 +87186,7 @@
         <v>1163</v>
       </c>
       <c r="D2203" s="1" t="s">
-        <v>9224</v>
+        <v>9223</v>
       </c>
       <c r="E2203" s="1" t="s">
         <v>5949</v>
@@ -87403,7 +87403,7 @@
         <v>7</v>
       </c>
       <c r="D2214" s="1" t="s">
-        <v>9183</v>
+        <v>9182</v>
       </c>
       <c r="E2214" s="1" t="s">
         <v>5821</v>
@@ -87420,7 +87420,7 @@
         <v>7</v>
       </c>
       <c r="D2215" s="1" t="s">
-        <v>9184</v>
+        <v>9183</v>
       </c>
       <c r="E2215" s="1" t="s">
         <v>5824</v>
@@ -87708,7 +87708,7 @@
         <v>7</v>
       </c>
       <c r="D2230" s="1" t="s">
-        <v>9185</v>
+        <v>9184</v>
       </c>
       <c r="E2230" s="1" t="s">
         <v>5827</v>
@@ -88165,7 +88165,7 @@
         <v>6804</v>
       </c>
       <c r="D2253" s="1" t="s">
-        <v>9325</v>
+        <v>9324</v>
       </c>
       <c r="E2253" s="1" t="s">
         <v>6825</v>
@@ -88182,7 +88182,7 @@
         <v>6804</v>
       </c>
       <c r="D2254" s="1" t="s">
-        <v>9327</v>
+        <v>9326</v>
       </c>
       <c r="E2254" s="1" t="s">
         <v>6831</v>
@@ -88199,7 +88199,7 @@
         <v>6804</v>
       </c>
       <c r="D2255" s="1" t="s">
-        <v>9326</v>
+        <v>9325</v>
       </c>
       <c r="E2255" s="1" t="s">
         <v>6828</v>
@@ -88216,7 +88216,7 @@
         <v>7</v>
       </c>
       <c r="D2256" s="1" t="s">
-        <v>9186</v>
+        <v>9185</v>
       </c>
       <c r="E2256" s="1" t="s">
         <v>5830</v>
@@ -88233,7 +88233,7 @@
         <v>7</v>
       </c>
       <c r="D2257" s="1" t="s">
-        <v>9187</v>
+        <v>9186</v>
       </c>
       <c r="E2257" s="1" t="s">
         <v>5833</v>
@@ -88250,7 +88250,7 @@
         <v>7</v>
       </c>
       <c r="D2258" s="1" t="s">
-        <v>9188</v>
+        <v>9187</v>
       </c>
       <c r="E2258" s="1" t="s">
         <v>5836</v>
@@ -88387,7 +88387,7 @@
         <v>3085</v>
       </c>
       <c r="D2265" s="1" t="s">
-        <v>9418</v>
+        <v>9417</v>
       </c>
       <c r="E2265" s="1" t="s">
         <v>7121</v>
@@ -88404,7 +88404,7 @@
         <v>3085</v>
       </c>
       <c r="D2266" s="1" t="s">
-        <v>9419</v>
+        <v>9418</v>
       </c>
       <c r="E2266" s="1" t="s">
         <v>7124</v>
@@ -88458,7 +88458,7 @@
         <v>7</v>
       </c>
       <c r="D2269" s="1" t="s">
-        <v>9189</v>
+        <v>9188</v>
       </c>
       <c r="E2269" s="1" t="s">
         <v>5839</v>
@@ -88475,7 +88475,7 @@
         <v>7</v>
       </c>
       <c r="D2270" s="1" t="s">
-        <v>9190</v>
+        <v>9189</v>
       </c>
       <c r="E2270" s="1" t="s">
         <v>5841</v>
@@ -88492,7 +88492,7 @@
         <v>7</v>
       </c>
       <c r="D2271" s="1" t="s">
-        <v>9191</v>
+        <v>9190</v>
       </c>
       <c r="E2271" s="1" t="s">
         <v>5844</v>
@@ -88649,7 +88649,7 @@
         <v>2957</v>
       </c>
       <c r="D2279" s="1" t="s">
-        <v>9467</v>
+        <v>9466</v>
       </c>
       <c r="E2279" s="1" t="s">
         <v>3225</v>
@@ -88666,7 +88666,7 @@
         <v>281</v>
       </c>
       <c r="D2280" s="1" t="s">
-        <v>9192</v>
+        <v>9191</v>
       </c>
       <c r="E2280" s="1" t="s">
         <v>5848</v>
@@ -88740,7 +88740,7 @@
         <v>3445</v>
       </c>
       <c r="D2284" s="1" t="s">
-        <v>9541</v>
+        <v>9540</v>
       </c>
       <c r="E2284" s="1" t="s">
         <v>3571</v>
@@ -88777,7 +88777,7 @@
         <v>692</v>
       </c>
       <c r="D2286" s="1" t="s">
-        <v>9516</v>
+        <v>9515</v>
       </c>
       <c r="E2286" s="1" t="s">
         <v>693</v>
@@ -88834,7 +88834,7 @@
         <v>885</v>
       </c>
       <c r="D2289" s="1" t="s">
-        <v>9366</v>
+        <v>9365</v>
       </c>
       <c r="E2289" s="1" t="s">
         <v>6939</v>
@@ -88851,7 +88851,7 @@
         <v>7</v>
       </c>
       <c r="D2290" s="1" t="s">
-        <v>9193</v>
+        <v>9192</v>
       </c>
       <c r="E2290" s="1" t="s">
         <v>5854</v>
@@ -88868,7 +88868,7 @@
         <v>7</v>
       </c>
       <c r="D2291" s="1" t="s">
-        <v>9194</v>
+        <v>9193</v>
       </c>
       <c r="E2291" s="1" t="s">
         <v>5856</v>
@@ -88885,7 +88885,7 @@
         <v>7</v>
       </c>
       <c r="D2292" s="1" t="s">
-        <v>9195</v>
+        <v>9194</v>
       </c>
       <c r="E2292" s="1" t="s">
         <v>5859</v>
@@ -88982,7 +88982,7 @@
         <v>7</v>
       </c>
       <c r="D2297" s="1" t="s">
-        <v>9196</v>
+        <v>9195</v>
       </c>
       <c r="E2297" s="1" t="s">
         <v>5861</v>
@@ -89059,7 +89059,7 @@
         <v>1950</v>
       </c>
       <c r="D2301" s="1" t="s">
-        <v>9423</v>
+        <v>9422</v>
       </c>
       <c r="E2301" s="1" t="s">
         <v>7136</v>
@@ -89076,7 +89076,7 @@
         <v>7</v>
       </c>
       <c r="D2302" s="1" t="s">
-        <v>9197</v>
+        <v>9196</v>
       </c>
       <c r="E2302" s="1" t="s">
         <v>5864</v>
@@ -89153,7 +89153,7 @@
         <v>7</v>
       </c>
       <c r="D2306" s="1" t="s">
-        <v>9198</v>
+        <v>9197</v>
       </c>
       <c r="E2306" s="1" t="s">
         <v>5866</v>
@@ -89170,7 +89170,7 @@
         <v>7</v>
       </c>
       <c r="D2307" s="1" t="s">
-        <v>9203</v>
+        <v>9202</v>
       </c>
       <c r="E2307" s="1" t="s">
         <v>5882</v>
@@ -89207,7 +89207,7 @@
         <v>7</v>
       </c>
       <c r="D2309" s="1" t="s">
-        <v>9204</v>
+        <v>9203</v>
       </c>
       <c r="E2309" s="1" t="s">
         <v>5885</v>
@@ -89244,7 +89244,7 @@
         <v>1950</v>
       </c>
       <c r="D2311" s="1" t="s">
-        <v>9422</v>
+        <v>9421</v>
       </c>
       <c r="E2311" s="1" t="s">
         <v>7133</v>
@@ -89261,7 +89261,7 @@
         <v>7</v>
       </c>
       <c r="D2312" s="1" t="s">
-        <v>9205</v>
+        <v>9204</v>
       </c>
       <c r="E2312" s="1" t="s">
         <v>5888</v>
@@ -89298,7 +89298,7 @@
         <v>1335</v>
       </c>
       <c r="D2314" s="1" t="s">
-        <v>9200</v>
+        <v>9199</v>
       </c>
       <c r="E2314" s="1" t="s">
         <v>5872</v>
@@ -89315,7 +89315,7 @@
         <v>1182</v>
       </c>
       <c r="D2315" s="1" t="s">
-        <v>9199</v>
+        <v>9198</v>
       </c>
       <c r="E2315" s="1" t="s">
         <v>5869</v>
@@ -89332,7 +89332,7 @@
         <v>7</v>
       </c>
       <c r="D2316" s="1" t="s">
-        <v>9206</v>
+        <v>9205</v>
       </c>
       <c r="E2316" s="1" t="s">
         <v>5891</v>
@@ -89349,7 +89349,7 @@
         <v>7</v>
       </c>
       <c r="D2317" s="1" t="s">
-        <v>9207</v>
+        <v>9206</v>
       </c>
       <c r="E2317" s="1" t="s">
         <v>5894</v>
@@ -89366,7 +89366,7 @@
         <v>7</v>
       </c>
       <c r="D2318" s="1" t="s">
-        <v>9208</v>
+        <v>9207</v>
       </c>
       <c r="E2318" s="1" t="s">
         <v>5898</v>
@@ -89383,7 +89383,7 @@
         <v>5616</v>
       </c>
       <c r="D2319" s="1" t="s">
-        <v>9202</v>
+        <v>9201</v>
       </c>
       <c r="E2319" s="1" t="s">
         <v>5879</v>
@@ -89440,7 +89440,7 @@
         <v>7</v>
       </c>
       <c r="D2322" s="1" t="s">
-        <v>9209</v>
+        <v>9208</v>
       </c>
       <c r="E2322" s="1" t="s">
         <v>5900</v>
@@ -89514,7 +89514,7 @@
         <v>5875</v>
       </c>
       <c r="D2326" s="1" t="s">
-        <v>9201</v>
+        <v>9200</v>
       </c>
       <c r="E2326" s="1" t="s">
         <v>5876</v>
@@ -89551,7 +89551,7 @@
         <v>7</v>
       </c>
       <c r="D2328" s="1" t="s">
-        <v>9210</v>
+        <v>9209</v>
       </c>
       <c r="E2328" s="1" t="s">
         <v>5904</v>
@@ -89588,7 +89588,7 @@
         <v>7</v>
       </c>
       <c r="D2330" s="1" t="s">
-        <v>9211</v>
+        <v>9210</v>
       </c>
       <c r="E2330" s="1" t="s">
         <v>5907</v>
@@ -89605,7 +89605,7 @@
         <v>1047</v>
       </c>
       <c r="D2331" s="1" t="s">
-        <v>9368</v>
+        <v>9367</v>
       </c>
       <c r="E2331" s="1" t="s">
         <v>6945</v>
@@ -89702,7 +89702,7 @@
         <v>7</v>
       </c>
       <c r="D2336" s="1" t="s">
-        <v>9212</v>
+        <v>9211</v>
       </c>
       <c r="E2336" s="1" t="s">
         <v>5910</v>
@@ -89779,7 +89779,7 @@
         <v>7</v>
       </c>
       <c r="D2340" s="1" t="s">
-        <v>9213</v>
+        <v>9212</v>
       </c>
       <c r="E2340" s="1" t="s">
         <v>5913</v>
@@ -89816,7 +89816,7 @@
         <v>7</v>
       </c>
       <c r="D2342" s="1" t="s">
-        <v>9214</v>
+        <v>9213</v>
       </c>
       <c r="E2342" s="1" t="s">
         <v>5916</v>
@@ -89833,7 +89833,7 @@
         <v>7</v>
       </c>
       <c r="D2343" s="1" t="s">
-        <v>9215</v>
+        <v>9214</v>
       </c>
       <c r="E2343" s="1" t="s">
         <v>5918</v>
@@ -89890,7 +89890,7 @@
         <v>217</v>
       </c>
       <c r="D2346" s="1" t="s">
-        <v>9316</v>
+        <v>9315</v>
       </c>
       <c r="E2346" s="1" t="s">
         <v>6794</v>
@@ -89927,7 +89927,7 @@
         <v>7</v>
       </c>
       <c r="D2348" s="1" t="s">
-        <v>9216</v>
+        <v>9215</v>
       </c>
       <c r="E2348" s="1" t="s">
         <v>5920</v>
@@ -89947,7 +89947,7 @@
         <v>4445</v>
       </c>
       <c r="D2349" t="s">
-        <v>9399</v>
+        <v>9398</v>
       </c>
       <c r="E2349" t="s">
         <v>7059</v>
@@ -89967,7 +89967,7 @@
         <v>4445</v>
       </c>
       <c r="D2350" s="1" t="s">
-        <v>9398</v>
+        <v>9397</v>
       </c>
       <c r="E2350" s="1" t="s">
         <v>7056</v>
@@ -90021,7 +90021,7 @@
         <v>974</v>
       </c>
       <c r="D2353" s="1" t="s">
-        <v>9369</v>
+        <v>9368</v>
       </c>
       <c r="E2353" s="1" t="s">
         <v>6948</v>
@@ -90092,7 +90092,7 @@
         <v>7</v>
       </c>
       <c r="D2357" s="1" t="s">
-        <v>9217</v>
+        <v>9216</v>
       </c>
       <c r="E2357" s="1" t="s">
         <v>5926</v>
@@ -90446,7 +90446,7 @@
         <v>4373</v>
       </c>
       <c r="D2375" s="1" t="s">
-        <v>9094</v>
+        <v>9093</v>
       </c>
       <c r="E2375" s="1" t="s">
         <v>4385</v>
@@ -90466,7 +90466,7 @@
         <v>4373</v>
       </c>
       <c r="D2376" s="1" t="s">
-        <v>9094</v>
+        <v>9093</v>
       </c>
       <c r="E2376" s="1" t="s">
         <v>4385</v>
@@ -90566,7 +90566,7 @@
         <v>4373</v>
       </c>
       <c r="D2381" s="1" t="s">
-        <v>9517</v>
+        <v>9516</v>
       </c>
       <c r="E2381" s="1" t="s">
         <v>4388</v>
@@ -90683,7 +90683,7 @@
         <v>7150</v>
       </c>
       <c r="D2387" s="1" t="s">
-        <v>9428</v>
+        <v>9427</v>
       </c>
       <c r="E2387" s="1" t="s">
         <v>7151</v>
@@ -90700,7 +90700,7 @@
         <v>7</v>
       </c>
       <c r="D2388" s="1" t="s">
-        <v>9218</v>
+        <v>9217</v>
       </c>
       <c r="E2388" s="1" t="s">
         <v>5932</v>
@@ -90737,7 +90737,7 @@
         <v>7</v>
       </c>
       <c r="D2390" s="4" t="s">
-        <v>9219</v>
+        <v>9218</v>
       </c>
       <c r="E2390" s="4" t="s">
         <v>5935</v>
@@ -90794,7 +90794,7 @@
         <v>7</v>
       </c>
       <c r="D2393" s="1" t="s">
-        <v>9220</v>
+        <v>9219</v>
       </c>
       <c r="E2393" s="1" t="s">
         <v>5938</v>
@@ -90831,7 +90831,7 @@
         <v>7</v>
       </c>
       <c r="D2395" s="1" t="s">
-        <v>9221</v>
+        <v>9220</v>
       </c>
       <c r="E2395" s="1" t="s">
         <v>5941</v>
@@ -90868,7 +90868,7 @@
         <v>7</v>
       </c>
       <c r="D2397" s="1" t="s">
-        <v>9222</v>
+        <v>9221</v>
       </c>
       <c r="E2397" s="1" t="s">
         <v>5944</v>
@@ -90945,7 +90945,7 @@
         <v>7</v>
       </c>
       <c r="D2401" s="1" t="s">
-        <v>9223</v>
+        <v>9222</v>
       </c>
       <c r="E2401" s="1" t="s">
         <v>5947</v>
@@ -91002,7 +91002,7 @@
         <v>7</v>
       </c>
       <c r="D2404" s="1" t="s">
-        <v>9225</v>
+        <v>9224</v>
       </c>
       <c r="E2404" s="1" t="s">
         <v>5952</v>
@@ -91019,7 +91019,7 @@
         <v>3380</v>
       </c>
       <c r="D2405" s="1" t="s">
-        <v>9357</v>
+        <v>9356</v>
       </c>
       <c r="E2405" s="1" t="s">
         <v>6921</v>
@@ -91150,7 +91150,7 @@
         <v>7</v>
       </c>
       <c r="D2412" s="1" t="s">
-        <v>9226</v>
+        <v>9225</v>
       </c>
       <c r="E2412" s="1" t="s">
         <v>5960</v>
@@ -91167,7 +91167,7 @@
         <v>46</v>
       </c>
       <c r="D2413" s="1" t="s">
-        <v>9227</v>
+        <v>9226</v>
       </c>
       <c r="E2413" s="1" t="s">
         <v>3459</v>
@@ -91221,7 +91221,7 @@
         <v>7</v>
       </c>
       <c r="D2416" s="1" t="s">
-        <v>9228</v>
+        <v>9227</v>
       </c>
       <c r="E2416" s="1" t="s">
         <v>5965</v>
@@ -91315,7 +91315,7 @@
         <v>7</v>
       </c>
       <c r="D2421" s="1" t="s">
-        <v>9229</v>
+        <v>9228</v>
       </c>
       <c r="E2421" s="1" t="s">
         <v>5969</v>
@@ -91332,7 +91332,7 @@
         <v>7</v>
       </c>
       <c r="D2422" s="1" t="s">
-        <v>9230</v>
+        <v>9229</v>
       </c>
       <c r="E2422" s="1" t="s">
         <v>5972</v>
@@ -91366,7 +91366,7 @@
         <v>7</v>
       </c>
       <c r="D2424" s="1" t="s">
-        <v>9231</v>
+        <v>9230</v>
       </c>
       <c r="E2424" s="1" t="s">
         <v>5975</v>
@@ -91383,7 +91383,7 @@
         <v>7</v>
       </c>
       <c r="D2425" s="1" t="s">
-        <v>9232</v>
+        <v>9231</v>
       </c>
       <c r="E2425" s="1" t="s">
         <v>5978</v>
@@ -91520,7 +91520,7 @@
         <v>46</v>
       </c>
       <c r="D2432" s="1" t="s">
-        <v>9233</v>
+        <v>9232</v>
       </c>
       <c r="E2432" s="1" t="s">
         <v>5985</v>
@@ -91537,7 +91537,7 @@
         <v>3234</v>
       </c>
       <c r="D2433" s="1" t="s">
-        <v>9234</v>
+        <v>9233</v>
       </c>
       <c r="E2433" s="1" t="s">
         <v>5987</v>
@@ -91554,7 +91554,7 @@
         <v>7</v>
       </c>
       <c r="D2434" s="1" t="s">
-        <v>9235</v>
+        <v>9234</v>
       </c>
       <c r="E2434" s="1" t="s">
         <v>5992</v>
@@ -91625,7 +91625,7 @@
         <v>7</v>
       </c>
       <c r="D2438" s="1" t="s">
-        <v>9236</v>
+        <v>9235</v>
       </c>
       <c r="E2438" s="1" t="s">
         <v>5995</v>
@@ -91642,7 +91642,7 @@
         <v>46</v>
       </c>
       <c r="D2439" s="1" t="s">
-        <v>9185</v>
+        <v>9184</v>
       </c>
       <c r="E2439" s="1" t="s">
         <v>5827</v>
@@ -91679,7 +91679,7 @@
         <v>710</v>
       </c>
       <c r="D2441" s="1" t="s">
-        <v>9518</v>
+        <v>9517</v>
       </c>
       <c r="E2441" s="1" t="s">
         <v>6638</v>
@@ -91699,7 +91699,7 @@
         <v>710</v>
       </c>
       <c r="D2442" s="1" t="s">
-        <v>9519</v>
+        <v>9518</v>
       </c>
       <c r="E2442" s="1" t="s">
         <v>6632</v>
@@ -91719,7 +91719,7 @@
         <v>710</v>
       </c>
       <c r="D2443" s="1" t="s">
-        <v>9520</v>
+        <v>9519</v>
       </c>
       <c r="E2443" s="1" t="s">
         <v>6635</v>
@@ -91736,7 +91736,7 @@
         <v>7</v>
       </c>
       <c r="D2444" s="1" t="s">
-        <v>9237</v>
+        <v>9236</v>
       </c>
       <c r="E2444" s="1" t="s">
         <v>5998</v>
@@ -91753,7 +91753,7 @@
         <v>7</v>
       </c>
       <c r="D2445" s="1" t="s">
-        <v>9238</v>
+        <v>9237</v>
       </c>
       <c r="E2445" s="1" t="s">
         <v>6001</v>
@@ -91770,7 +91770,7 @@
         <v>7</v>
       </c>
       <c r="D2446" s="1" t="s">
-        <v>9239</v>
+        <v>9238</v>
       </c>
       <c r="E2446" s="1" t="s">
         <v>6004</v>
@@ -91787,7 +91787,7 @@
         <v>7</v>
       </c>
       <c r="D2447" s="1" t="s">
-        <v>9240</v>
+        <v>9239</v>
       </c>
       <c r="E2447" s="1" t="s">
         <v>6007</v>
@@ -91984,7 +91984,7 @@
         <v>1378</v>
       </c>
       <c r="D2457" s="4" t="s">
-        <v>9440</v>
+        <v>9439</v>
       </c>
       <c r="E2457" s="4" t="s">
         <v>7191</v>
@@ -92121,7 +92121,7 @@
         <v>7</v>
       </c>
       <c r="D2464" s="1" t="s">
-        <v>9241</v>
+        <v>9240</v>
       </c>
       <c r="E2464" s="1" t="s">
         <v>6010</v>
@@ -93492,7 +93492,7 @@
         <v>7</v>
       </c>
       <c r="D2533" s="1" t="s">
-        <v>9243</v>
+        <v>9242</v>
       </c>
       <c r="E2533" s="1" t="s">
         <v>6016</v>
@@ -93569,7 +93569,7 @@
         <v>2795</v>
       </c>
       <c r="D2537" s="1" t="s">
-        <v>9521</v>
+        <v>9520</v>
       </c>
       <c r="E2537" s="1" t="s">
         <v>22</v>
@@ -93743,7 +93743,7 @@
         <v>7</v>
       </c>
       <c r="D2546" s="1" t="s">
-        <v>9245</v>
+        <v>9244</v>
       </c>
       <c r="E2546" s="1" t="s">
         <v>6023</v>
@@ -93800,7 +93800,7 @@
         <v>7</v>
       </c>
       <c r="D2549" s="1" t="s">
-        <v>9246</v>
+        <v>9245</v>
       </c>
       <c r="E2549" s="1" t="s">
         <v>6026</v>
@@ -93871,7 +93871,7 @@
         <v>252</v>
       </c>
       <c r="D2553" s="1" t="s">
-        <v>9411</v>
+        <v>9410</v>
       </c>
       <c r="E2553" s="1" t="s">
         <v>7096</v>
@@ -94002,7 +94002,7 @@
         <v>3780</v>
       </c>
       <c r="D2560" s="1" t="s">
-        <v>9522</v>
+        <v>9521</v>
       </c>
       <c r="E2560" s="1" t="s">
         <v>3790</v>

</xml_diff>